<commit_message>
Add functionality to save data to Excel and upload to AWS S3
- Implement save_to_excel function to save product data to an Excel file
- Integrate AWS S3 to upload the Excel file to a specified bucket
- Add Streamlit interface elements to display success and error messages
- Include AWS S3 connection and file upload logic

This commit enhances the application by adding the ability to save search results to an Excel file and upload it to AWS S3 for storage.
</commit_message>
<xml_diff>
--- a/products.xlsx
+++ b/products.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:E91"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -730,6 +730,2166 @@
         </is>
       </c>
     </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>2025-03-11</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>GIGABYTE Z790 Aorus Elite AX (LGA 1700/ Intel Z790/ ATX/ DDR5/Quad M.2/PCIe 5.0/USB 3.2 Gen2X2 Tipo C/Intel WiFi 6E/LAN de 2.5GbE/Q-Flash Plus/PCIe EZ-Latch/placa base para juegos)</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Página 1 de 1  </t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>https://m.media-amazon.com/images/I/81a48Z1GciL.__AC_SY300_SX300_QL70_ML2_.jpg</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com/-/es/GIGABYTE-Z790-AX-Q-Flash-EZ-Latch/dp/B0BH9DXY38/ref=sr_1_1?dib=eyJ2IjoiMSJ9.MqH-CQnxBqi5Kkr0pAwc_FeTsRBVBHfe3orT1xyvNb2JvTnFxJ47pTrKiCQ0qruW0D7a68DFh_Io3P5V5l3rHJWySOvdGkArmkcPzmVf2so5BTMLKGOHkvejOCeZD-mOWWIwAWqDfG6s2OQkHzHHdXZOMfwnRqR6vgxewE_Uv-nbfr1-UeiiJ5yXXmaNkhbgbEs55VAFdurjBCC-w7xIHn2OiVnobAaWmUYZG7svEVM.b6SoKH_nsH7kCZMGLo7hnPqrZQPUPXuCEuM91qcI7mQ&amp;dib_tag=se&amp;keywords=Z790+AORUS&amp;qid=1741742704&amp;sr=8-1</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>2025-03-11</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>GIGABYTE Z790 AORUS PRO X WIFI7 LGA 1700 Intel Z790 X ATX placa base con DDR5, 5* M.2, PCIe 5.0, USB 3.2 Tipo-C, Wi-Fi 7, LAN de 5GbE, Q-Flash Plus, EZ-Latch Plus</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>US$260.76</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>https://m.media-amazon.com/images/I/71jwye+xDLL._AC_SX300_SY300_.jpg</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com/-/es/GIGABYTE-Z790-AORUS-PRO-WIFI7/dp/B0CTTVFWHM/ref=sr_1_2?dib=eyJ2IjoiMSJ9.MqH-CQnxBqi5Kkr0pAwc_FeTsRBVBHfe3orT1xyvNb2JvTnFxJ47pTrKiCQ0qruW0D7a68DFh_Io3P5V5l3rHJWySOvdGkArmkcPzmVf2so5BTMLKGOHkvejOCeZD-mOWWIwAWqDfG6s2OQkHzHHdXZOMfwnRqR6vgxewE_Uv-nbfr1-UeiiJ5yXXmaNkhbgbEs55VAFdurjBCC-w7xIHn2OiVnobAaWmUYZG7svEVM.b6SoKH_nsH7kCZMGLo7hnPqrZQPUPXuCEuM91qcI7mQ&amp;dib_tag=se&amp;keywords=Z790+AORUS&amp;qid=1741742704&amp;sr=8-2</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>2025-03-11</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>GIGABYTE Z790 AORUS PRO X (LGA 1700/ Intel/ Z790 X/ATX/ DDR5/ 5* M.2/PCIe 5.0/USB 3.2 Tipo-C/Wi-Fi 7/LAN de 5GbE/Q-Flash Plus/EZ-Latch Plus/Placa base)</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>US$329.99</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>https://m.media-amazon.com/images/I/71lzIrBDJtL.__AC_SY300_SX300_QL70_ML2_.jpg</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com/-/es/GIGABYTE-Z790-AORUS-PRO-EZ-Latch/dp/B083RW9TJF/ref=sr_1_3?dib=eyJ2IjoiMSJ9.MqH-CQnxBqi5Kkr0pAwc_FeTsRBVBHfe3orT1xyvNb2JvTnFxJ47pTrKiCQ0qruW0D7a68DFh_Io3P5V5l3rHJWySOvdGkArmkcPzmVf2so5BTMLKGOHkvejOCeZD-mOWWIwAWqDfG6s2OQkHzHHdXZOMfwnRqR6vgxewE_Uv-nbfr1-UeiiJ5yXXmaNkhbgbEs55VAFdurjBCC-w7xIHn2OiVnobAaWmUYZG7svEVM.b6SoKH_nsH7kCZMGLo7hnPqrZQPUPXuCEuM91qcI7mQ&amp;dib_tag=se&amp;keywords=Z790+AORUS&amp;qid=1741742704&amp;sr=8-3</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>2025-03-11</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>GIGABYTE Z790 AORUS Elite AX 1.0 Intel LGA 1700 ATX placa base, 4X DDR5~128GB, 3X PCI-E x16, 4X M.2, 6X SATA, 5X USB 3.2, 1x USB-C, 4X USB 2.0</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>US$209.99</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>https://m.media-amazon.com/images/I/61T1P18owDL.__AC_SX300_SY300_QL70_ML2_.jpg</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com/-/es/GIGABYTE-Z790-AORUS-AX-DDR5-128GB/dp/B0BH28M64J/ref=sr_1_4?dib=eyJ2IjoiMSJ9.MqH-CQnxBqi5Kkr0pAwc_FeTsRBVBHfe3orT1xyvNb2JvTnFxJ47pTrKiCQ0qruW0D7a68DFh_Io3P5V5l3rHJWySOvdGkArmkcPzmVf2so5BTMLKGOHkvejOCeZD-mOWWIwAWqDfG6s2OQkHzHHdXZOMfwnRqR6vgxewE_Uv-nbfr1-UeiiJ5yXXmaNkhbgbEs55VAFdurjBCC-w7xIHn2OiVnobAaWmUYZG7svEVM.b6SoKH_nsH7kCZMGLo7hnPqrZQPUPXuCEuM91qcI7mQ&amp;dib_tag=se&amp;keywords=Z790+AORUS&amp;qid=1741742704&amp;sr=8-4</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>2025-03-11</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>GIGABYTE Z790I AORUS Ultra (LGA 1700/ Intel/ Z790/ Mini-ITX/ DDR5/ Dual M.2/ PCIe 5.0/ USB 3.2 Gen2X2 Tipo C/Intel Killer Wi-Fi 6E/Intel 2.5GbE LAN/Q-Flash Plus/placa madre)</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>US$312.70</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>https://m.media-amazon.com/images/I/81EwpyGT29L.__AC_SY300_SX300_QL70_ML2_.jpg</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com/-/es/GIGABYTE-Z790I-AORUS-Mini-ITX-Q-Flash/dp/B0BZQ43XXL/ref=sr_1_5?dib=eyJ2IjoiMSJ9.MqH-CQnxBqi5Kkr0pAwc_FeTsRBVBHfe3orT1xyvNb2JvTnFxJ47pTrKiCQ0qruW0D7a68DFh_Io3P5V5l3rHJWySOvdGkArmkcPzmVf2so5BTMLKGOHkvejOCeZD-mOWWIwAWqDfG6s2OQkHzHHdXZOMfwnRqR6vgxewE_Uv-nbfr1-UeiiJ5yXXmaNkhbgbEs55VAFdurjBCC-w7xIHn2OiVnobAaWmUYZG7svEVM.b6SoKH_nsH7kCZMGLo7hnPqrZQPUPXuCEuM91qcI7mQ&amp;dib_tag=se&amp;keywords=Z790+AORUS&amp;qid=1741742704&amp;sr=8-5</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>2025-03-11</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>ASUS TUF Gaming Z790-Plus WiFi LGA 1700 (Intel 14ª, 12ª y 13ª generación) ATX placa base para juegos (PCIe 5.0, DDR5, 4xM.2 ranuras, 16+1 DrMOS, WiFi 6, LAN de 2.5 Gb, USB frontal 3.2 Gen 2 tipo C,</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>US$199.00</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>https://m.media-amazon.com/images/I/81rX0VhoStL.__AC_SX300_SY300_QL70_ML2_.jpg</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com/-/es/TUF-Z790-Plus-generaci%C3%B3n-ranuras-frontal/dp/B0BQD58D96/ref=sr_1_6?dib=eyJ2IjoiMSJ9.MqH-CQnxBqi5Kkr0pAwc_FeTsRBVBHfe3orT1xyvNb2JvTnFxJ47pTrKiCQ0qruW0D7a68DFh_Io3P5V5l3rHJWySOvdGkArmkcPzmVf2so5BTMLKGOHkvejOCeZD-mOWWIwAWqDfG6s2OQkHzHHdXZOMfwnRqR6vgxewE_Uv-nbfr1-UeiiJ5yXXmaNkhbgbEs55VAFdurjBCC-w7xIHn2OiVnobAaWmUYZG7svEVM.b6SoKH_nsH7kCZMGLo7hnPqrZQPUPXuCEuM91qcI7mQ&amp;dib_tag=se&amp;keywords=Z790+AORUS&amp;qid=1741742704&amp;sr=8-6</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>2025-03-11</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>GIGABYTE Z790 AORUS ELITE DDR4 Intel LGA 1700 ATX placa base, 4 x DDR4 ~ 128GB, 3x PCI-E x16, 4x M.2, 4x SATA, 5x USB 3.2, 1x USB-C, 4x USB 2.0</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>US$248.71</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>https://m.media-amazon.com/images/I/61iiVI3vTfL.__AC_SX300_SY300_QL70_ML2_.jpg</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com/-/es/GIGABYTE-Z790-AORUS-ELITE-DDR4/dp/B0BPMGC4RJ/ref=sr_1_7?dib=eyJ2IjoiMSJ9.MqH-CQnxBqi5Kkr0pAwc_FeTsRBVBHfe3orT1xyvNb2JvTnFxJ47pTrKiCQ0qruW0D7a68DFh_Io3P5V5l3rHJWySOvdGkArmkcPzmVf2so5BTMLKGOHkvejOCeZD-mOWWIwAWqDfG6s2OQkHzHHdXZOMfwnRqR6vgxewE_Uv-nbfr1-UeiiJ5yXXmaNkhbgbEs55VAFdurjBCC-w7xIHn2OiVnobAaWmUYZG7svEVM.b6SoKH_nsH7kCZMGLo7hnPqrZQPUPXuCEuM91qcI7mQ&amp;dib_tag=se&amp;keywords=Z790+AORUS&amp;qid=1741742704&amp;sr=8-7</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>2025-03-11</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>GIGABYTE Z790 Gaming Plus AX LGA 1700 Intel Z790 ATX placa base con DDR5, Triple M.2, PCIe 4.0, USB 3.2 Gen2 Type-C, Realtek Wi-Fi 6, Realtek LAN, Q-Flash Plus, EZ-Latch</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>US$169.99</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>https://m.media-amazon.com/images/I/81Ip3DnEazL.__AC_SX300_SY300_QL70_ML2_.jpg</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com/-/es/GIGABYTE-Z790-AX-Realtek-EZ-Latch/dp/B0D8WH39QJ/ref=sr_1_8?dib=eyJ2IjoiMSJ9.MqH-CQnxBqi5Kkr0pAwc_FeTsRBVBHfe3orT1xyvNb2JvTnFxJ47pTrKiCQ0qruW0D7a68DFh_Io3P5V5l3rHJWySOvdGkArmkcPzmVf2so5BTMLKGOHkvejOCeZD-mOWWIwAWqDfG6s2OQkHzHHdXZOMfwnRqR6vgxewE_Uv-nbfr1-UeiiJ5yXXmaNkhbgbEs55VAFdurjBCC-w7xIHn2OiVnobAaWmUYZG7svEVM.b6SoKH_nsH7kCZMGLo7hnPqrZQPUPXuCEuM91qcI7mQ&amp;dib_tag=se&amp;keywords=Z790+AORUS&amp;qid=1741742704&amp;sr=8-8</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>2025-03-11</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>GIGABYTE Z790 Gaming X AX (LGA 1700/Intel/Z790/ATX/DDR5/M.2/PCIe 5.0/USB 3.2 Gen2X2 Tipo C/Intel Wi-Fi 6E/2.5GbE LAN/Q-Flash Plus/EZ-Latch Plus/Placa base para juegos)</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>US$219.99</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>https://m.media-amazon.com/images/I/81B9SuZS68L.__AC_SY300_SX300_QL70_ML2_.jpg</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com/-/es/GIGABYTE-Z790-AX-Q-Flash-EZ-Latch/dp/B0BSVYXM5C/ref=sr_1_9?dib=eyJ2IjoiMSJ9.MqH-CQnxBqi5Kkr0pAwc_FeTsRBVBHfe3orT1xyvNb2JvTnFxJ47pTrKiCQ0qruW0D7a68DFh_Io3P5V5l3rHJWySOvdGkArmkcPzmVf2so5BTMLKGOHkvejOCeZD-mOWWIwAWqDfG6s2OQkHzHHdXZOMfwnRqR6vgxewE_Uv-nbfr1-UeiiJ5yXXmaNkhbgbEs55VAFdurjBCC-w7xIHn2OiVnobAaWmUYZG7svEVM.b6SoKH_nsH7kCZMGLo7hnPqrZQPUPXuCEuM91qcI7mQ&amp;dib_tag=se&amp;keywords=Z790+AORUS&amp;qid=1741742704&amp;sr=8-9</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>2025-03-11</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>GIGABYTE Z790 AORUS Elite AX ICE Placa base Intel LGA 1700 ATX, 4X DDR5~192GB, 3X PCI-E x16, 4X M.2, 6X SATA, 5X USB 3.2, 1x USB-C, 4X USB 2.0</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>US$340.27</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>https://m.media-amazon.com/images/I/81HhWIZUL4L.__AC_SY300_SX300_QL70_ML2_.jpg</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com/-/es/Z790-AORUS-AX-ICE-DDR5-192GB/dp/B0CK75LYD2/ref=sr_1_10?dib=eyJ2IjoiMSJ9.MqH-CQnxBqi5Kkr0pAwc_FeTsRBVBHfe3orT1xyvNb2JvTnFxJ47pTrKiCQ0qruW0D7a68DFh_Io3P5V5l3rHJWySOvdGkArmkcPzmVf2so5BTMLKGOHkvejOCeZD-mOWWIwAWqDfG6s2OQkHzHHdXZOMfwnRqR6vgxewE_Uv-nbfr1-UeiiJ5yXXmaNkhbgbEs55VAFdurjBCC-w7xIHn2OiVnobAaWmUYZG7svEVM.b6SoKH_nsH7kCZMGLo7hnPqrZQPUPXuCEuM91qcI7mQ&amp;dib_tag=se&amp;keywords=Z790+AORUS&amp;qid=1741742704&amp;sr=8-10</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>2025-03-11</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>MSI Tarjeta gráfica para juegos GeForce RTX 4090 Gaming X Trio 24G - 24 GB GDDR6X, 2595 MHz, PCI Express Gen 4, 384 bits, 3X DP v 1.4a, HDMI 2.1a (compatible con 4K y 8K HDR)</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Página 1 de 1  </t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>https://m.media-amazon.com/images/I/81KR0fO8WgL.__AC_SX300_SY300_QL70_ML2_.jpg</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com/-/es/Tarjeta-gr%C3%A1fica-juegos-GeForce-Gaming/dp/B09YCLG5PB/ref=sr_1_1?dib=eyJ2IjoiMSJ9.F4Gr1t-QOvk2g6zRXXeN5RIIXNwYPtR7vXGeo57wzkx5W3IU6tp8KTKGJbsiNB02Q777CCJXzJwOyQSH5X_y4sfBc7Kw5Sj3gT1vp4Kk2derk8jq7Vz0VrBigqwNidQieLRyxXqWNfql06IjV0V0rceIy4DY8YgWwIAqYOrOSF-0ja0Cw4Ka_zmxOd5NuLbixq_yh4M4CME3gantX0COnjzrfZ1fZvTmUtKM0csh4Y4.senQiy6rcRv5wx8uDfClH6JS91zEkerFWJFD0ell_zU&amp;dib_tag=se&amp;keywords=RX+4090&amp;qid=1741743051&amp;sr=8-1</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>2025-03-11</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>MINISFORUM Base DEG1 eGPU, estación de acoplamiento externa de GPU para RTX 4090, AMD RX 7900 XTX, carcasa eGPU Tarjeta gráfica Extensión Soporte ATX/SFX Standard Power, Oculink Expansion Graphics</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>US$99.90</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>https://m.media-amazon.com/images/I/61fZUjmWe+L._AC_SY300_SX300_.jpg</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com/-/es/MINISFORUM-estaci%C3%B3n-acoplamiento-Extensi%C3%B3n-Expansion/dp/B0DPGYKH7G/ref=sr_1_2?dib=eyJ2IjoiMSJ9.F4Gr1t-QOvk2g6zRXXeN5RIIXNwYPtR7vXGeo57wzkx5W3IU6tp8KTKGJbsiNB02Q777CCJXzJwOyQSH5X_y4sfBc7Kw5Sj3gT1vp4Kk2derk8jq7Vz0VrBigqwNidQieLRyxXqWNfql06IjV0V0rceIy4DY8YgWwIAqYOrOSF-0ja0Cw4Ka_zmxOd5NuLbixq_yh4M4CME3gantX0COnjzrfZ1fZvTmUtKM0csh4Y4.senQiy6rcRv5wx8uDfClH6JS91zEkerFWJFD0ell_zU&amp;dib_tag=se&amp;keywords=RX+4090&amp;qid=1741743051&amp;sr=8-2</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>2025-03-11</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>Soporte de soporte para tarjeta gráfica, soporte de soporte de caída de tarjeta de video, soporte de GPU (L, 2.913-4.724 in)</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>US$9.99</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>https://m.media-amazon.com/images/I/312BAnEbBmL.__AC_SX300_SY300_QL70_ML2_.jpg</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com/-/es/Soporte-soporte-tarjeta-gr%C3%A1fica-2-913-4-724/dp/B09FPJL1KY/ref=sr_1_3?dib=eyJ2IjoiMSJ9.F4Gr1t-QOvk2g6zRXXeN5RIIXNwYPtR7vXGeo57wzkx5W3IU6tp8KTKGJbsiNB02Q777CCJXzJwOyQSH5X_y4sfBc7Kw5Sj3gT1vp4Kk2derk8jq7Vz0VrBigqwNidQieLRyxXqWNfql06IjV0V0rceIy4DY8YgWwIAqYOrOSF-0ja0Cw4Ka_zmxOd5NuLbixq_yh4M4CME3gantX0COnjzrfZ1fZvTmUtKM0csh4Y4.senQiy6rcRv5wx8uDfClH6JS91zEkerFWJFD0ell_zU&amp;dib_tag=se&amp;keywords=RX+4090&amp;qid=1741743051&amp;sr=8-3</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>2025-03-11</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>Soporte de GPU, 2.75-4.52 pulgadas GPU Sag soporte con hoja antideslizante, soporte de GPU para evitar el hundimiento de la tarjeta gráfica (negro)</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>US$9.98</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>https://m.media-amazon.com/images/I/61RmFTb8ebL.__AC_SX300_SY300_QL70_ML2_.jpg</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com/-/es/Ausvrkkit-2-75-4-52-pulgadas-antideslizante-hundimiento/dp/B0B2WCTGFV/ref=sr_1_4?dib=eyJ2IjoiMSJ9.F4Gr1t-QOvk2g6zRXXeN5RIIXNwYPtR7vXGeo57wzkx5W3IU6tp8KTKGJbsiNB02Q777CCJXzJwOyQSH5X_y4sfBc7Kw5Sj3gT1vp4Kk2derk8jq7Vz0VrBigqwNidQieLRyxXqWNfql06IjV0V0rceIy4DY8YgWwIAqYOrOSF-0ja0Cw4Ka_zmxOd5NuLbixq_yh4M4CME3gantX0COnjzrfZ1fZvTmUtKM0csh4Y4.senQiy6rcRv5wx8uDfClH6JS91zEkerFWJFD0ell_zU&amp;dib_tag=se&amp;keywords=RX+4090&amp;qid=1741743051&amp;sr=8-4</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>2025-03-11</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>Soporte de GPU, soporte para tarjeta de video gráfica con altura ajustable, soporte anti hundimiento para tarjeta gráfica universal, soporte de GPU con imán y almohadilla de goma (negro)</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>US$6.99</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>https://m.media-amazon.com/images/I/71H7BANd7nL.__AC_SX300_SY300_QL70_ML2_.jpg</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com/-/es/Aivalas-ajustable-hundimiento-universal-almohadilla/dp/B0BPGJCLYR/ref=sr_1_5?dib=eyJ2IjoiMSJ9.F4Gr1t-QOvk2g6zRXXeN5RIIXNwYPtR7vXGeo57wzkx5W3IU6tp8KTKGJbsiNB02Q777CCJXzJwOyQSH5X_y4sfBc7Kw5Sj3gT1vp4Kk2derk8jq7Vz0VrBigqwNidQieLRyxXqWNfql06IjV0V0rceIy4DY8YgWwIAqYOrOSF-0ja0Cw4Ka_zmxOd5NuLbixq_yh4M4CME3gantX0COnjzrfZ1fZvTmUtKM0csh4Y4.senQiy6rcRv5wx8uDfClH6JS91zEkerFWJFD0ell_zU&amp;dib_tag=se&amp;keywords=RX+4090&amp;qid=1741743051&amp;sr=8-5</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>2025-03-11</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>ASUS ROG Herculx - Soporte antidesgarro para tarjeta gráfica (construcción de aleación de zinc maciza, fácil instalación sin herramientas, nivel de burbuja incluido, altura ajustable, amplia</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>Página 1 de 1</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>https://m.media-amazon.com/images/I/71m4QHLRzmL.__AC_SX300_SY300_QL70_ML2_.jpg</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com/-/es/ASUS-ROG-Herculx-antidesgarro-construcci%C3%B3n/dp/B0B173F6RM/ref=sr_1_6?dib=eyJ2IjoiMSJ9.F4Gr1t-QOvk2g6zRXXeN5RIIXNwYPtR7vXGeo57wzkx5W3IU6tp8KTKGJbsiNB02Q777CCJXzJwOyQSH5X_y4sfBc7Kw5Sj3gT1vp4Kk2derk8jq7Vz0VrBigqwNidQieLRyxXqWNfql06IjV0V0rceIy4DY8YgWwIAqYOrOSF-0ja0Cw4Ka_zmxOd5NuLbixq_yh4M4CME3gantX0COnjzrfZ1fZvTmUtKM0csh4Y4.senQiy6rcRv5wx8uDfClH6JS91zEkerFWJFD0ell_zU&amp;dib_tag=se&amp;keywords=RX+4090&amp;qid=1741743051&amp;sr=8-6</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>2025-03-11</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>Tarjeta gráfica externa GPU Dock con fuente de alimentación de 750 W, para nVidia Geforce RTX 4080 4090 3080 3090 AMD Radeon RX 6900 7900 6800 7800 XT XTX, adaptador PCIE adicional estación de</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>US$195.88</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>https://m.media-amazon.com/images/I/61e+kqQ547L._AC_SY300_SX300_.jpg</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com/-/es/Tarjeta-alimentaci%C3%B3n-adaptador-adicional-estaci%C3%B3n/dp/B0DH556Z51/ref=sr_1_7?dib=eyJ2IjoiMSJ9.F4Gr1t-QOvk2g6zRXXeN5RIIXNwYPtR7vXGeo57wzkx5W3IU6tp8KTKGJbsiNB02Q777CCJXzJwOyQSH5X_y4sfBc7Kw5Sj3gT1vp4Kk2derk8jq7Vz0VrBigqwNidQieLRyxXqWNfql06IjV0V0rceIy4DY8YgWwIAqYOrOSF-0ja0Cw4Ka_zmxOd5NuLbixq_yh4M4CME3gantX0COnjzrfZ1fZvTmUtKM0csh4Y4.senQiy6rcRv5wx8uDfClH6JS91zEkerFWJFD0ell_zU&amp;dib_tag=se&amp;keywords=RX+4090&amp;qid=1741743051&amp;sr=8-7</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>2025-03-11</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>LINKUP - Cable elevador AVA5 PCIE 5.0 | RTX5090 5080 GPU Ready | Velocidad x16 128GB/s | Compatible con PCIe 4.0 y WRX80/WRX90E | Ángulo recto, negro 7.9 in</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>US$72.96</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>https://m.media-amazon.com/images/I/31utVuuP0GL._SY445_SX342_QL70_ML2_.jpg</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com/-/es/LINKUP-elevador-RTX5090-Velocidad-Compatible/dp/B0CXJKXN29/ref=sr_1_8?dib=eyJ2IjoiMSJ9.F4Gr1t-QOvk2g6zRXXeN5RIIXNwYPtR7vXGeo57wzkx5W3IU6tp8KTKGJbsiNB02Q777CCJXzJwOyQSH5X_y4sfBc7Kw5Sj3gT1vp4Kk2derk8jq7Vz0VrBigqwNidQieLRyxXqWNfql06IjV0V0rceIy4DY8YgWwIAqYOrOSF-0ja0Cw4Ka_zmxOd5NuLbixq_yh4M4CME3gantX0COnjzrfZ1fZvTmUtKM0csh4Y4.senQiy6rcRv5wx8uDfClH6JS91zEkerFWJFD0ell_zU&amp;dib_tag=se&amp;keywords=RX+4090&amp;qid=1741743051&amp;sr=8-8</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>2025-03-11</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>Cable Matters [Certificado VESA] Cable DisplayPort 2.1 de 80 Gbps - 6.6 pies, cable DP80 con 16K 60Hz, 8K 240Hz, 4K 240Hz, FreeSync, G-SYNC y HDR para monitor de juegos, PC, RTX 4080/4090, RX 7900,</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>US$15.99</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>https://m.media-amazon.com/images/I/41jZywVptuL._SY445_SX342_QL70_ML2_.jpg</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com/-/es/Cable-Matters-Certificado-VESA-DisplayPort/dp/B0DK5WYV8X/ref=sr_1_9?dib=eyJ2IjoiMSJ9.F4Gr1t-QOvk2g6zRXXeN5RIIXNwYPtR7vXGeo57wzkx5W3IU6tp8KTKGJbsiNB02Q777CCJXzJwOyQSH5X_y4sfBc7Kw5Sj3gT1vp4Kk2derk8jq7Vz0VrBigqwNidQieLRyxXqWNfql06IjV0V0rceIy4DY8YgWwIAqYOrOSF-0ja0Cw4Ka_zmxOd5NuLbixq_yh4M4CME3gantX0COnjzrfZ1fZvTmUtKM0csh4Y4.senQiy6rcRv5wx8uDfClH6JS91zEkerFWJFD0ell_zU&amp;dib_tag=se&amp;keywords=RX+4090&amp;qid=1741743051&amp;sr=8-9</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>2025-03-11</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>MINISFORUM DEG1 Estación de acoplamiento de GPU externa, mini gabinete eGPU para RTX 4090, AMD RX 7900 XTX, compatible con fuentes de alimentación estándar ATX/SFX, estación de base de gráficos de</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>US$129.90</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>https://m.media-amazon.com/images/I/51cs-T55DKL.__AC_SX300_SY300_QL70_ML2_.jpg</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com/-/es/MINISFORUM-Estaci%C3%B3n-acoplamiento-compatible-alimentaci%C3%B3n/dp/B0DCZLPWXK/ref=sr_1_10?dib=eyJ2IjoiMSJ9.F4Gr1t-QOvk2g6zRXXeN5RIIXNwYPtR7vXGeo57wzkx5W3IU6tp8KTKGJbsiNB02Q777CCJXzJwOyQSH5X_y4sfBc7Kw5Sj3gT1vp4Kk2derk8jq7Vz0VrBigqwNidQieLRyxXqWNfql06IjV0V0rceIy4DY8YgWwIAqYOrOSF-0ja0Cw4Ka_zmxOd5NuLbixq_yh4M4CME3gantX0COnjzrfZ1fZvTmUtKM0csh4Y4.senQiy6rcRv5wx8uDfClH6JS91zEkerFWJFD0ell_zU&amp;dib_tag=se&amp;keywords=RX+4090&amp;qid=1741743051&amp;sr=8-10</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>2025-03-11</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>MSI Tarjeta gráfica para juegos GeForce RTX 4090 Gaming X Trio 24G - 24 GB GDDR6X, 2595 MHz, PCI Express Gen 4, 384 bits, 3X DP v 1.4a, HDMI 2.1a (compatible con 4K y 8K HDR)</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Página 1 de 1  </t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>https://m.media-amazon.com/images/I/81KR0fO8WgL.__AC_SX300_SY300_QL70_ML2_.jpg</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com/-/es/Tarjeta-gr%C3%A1fica-juegos-GeForce-Gaming/dp/B09YCLG5PB/ref=sr_1_1?dib=eyJ2IjoiMSJ9.Sv4Tuv8E6sKBPCb3XoqbMVCKzyZMgVXH7YU1musRODLJFBXGrEv9WxoP-U667nNFme06I0FFm3k7Exv4qh0zQBoDXzuBk4ciQo-2z40Rtc9lWWDggXK5PjgXdQesu8XaxZBtZSq5jbVf1SlVMK1wiWDwpWRz-5xXxgc5Ba9UMKm2e2eoYxiamKujSp1LfbSm__G3KXx2LXPsZ0zbhDigwVToQ9yL9G3BrX055qA8ZdM.2pKjwTTa_MnITc-mxMd8Thc8rg1Yye3uWkY41IOngi8&amp;dib_tag=se&amp;keywords=RTX+4090+Ti&amp;qid=1741743897&amp;sr=8-1</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>2025-03-11</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>NVIDIA Quadro RTX 6000</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>US$2,339.00</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>https://m.media-amazon.com/images/I/41JfC7adkYL.__AC_SY300_SX300_QL70_ML2_.jpg</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com/-/es/VCQRTX6000-PB-NVIDIA-Quadro-RTX-6000/dp/B07HY86LMV/ref=sr_1_2?dib=eyJ2IjoiMSJ9.Sv4Tuv8E6sKBPCb3XoqbMVCKzyZMgVXH7YU1musRODLJFBXGrEv9WxoP-U667nNFme06I0FFm3k7Exv4qh0zQBoDXzuBk4ciQo-2z40Rtc9lWWDggXK5PjgXdQesu8XaxZBtZSq5jbVf1SlVMK1wiWDwpWRz-5xXxgc5Ba9UMKm2e2eoYxiamKujSp1LfbSm__G3KXx2LXPsZ0zbhDigwVToQ9yL9G3BrX055qA8ZdM.2pKjwTTa_MnITc-mxMd8Thc8rg1Yye3uWkY41IOngi8&amp;dib_tag=se&amp;keywords=RTX+4090+Ti&amp;qid=1741743897&amp;sr=8-2</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>2025-03-11</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>Soporte de soporte para tarjeta gráfica, soporte de soporte de caída de tarjeta de video, soporte de GPU (L, 2.913-4.724 in)</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>US$9.99</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>https://m.media-amazon.com/images/I/312BAnEbBmL.__AC_SX300_SY300_QL70_ML2_.jpg</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com/-/es/Soporte-soporte-tarjeta-gr%C3%A1fica-2-913-4-724/dp/B09FPJL1KY/ref=sr_1_3?dib=eyJ2IjoiMSJ9.Sv4Tuv8E6sKBPCb3XoqbMVCKzyZMgVXH7YU1musRODLJFBXGrEv9WxoP-U667nNFme06I0FFm3k7Exv4qh0zQBoDXzuBk4ciQo-2z40Rtc9lWWDggXK5PjgXdQesu8XaxZBtZSq5jbVf1SlVMK1wiWDwpWRz-5xXxgc5Ba9UMKm2e2eoYxiamKujSp1LfbSm__G3KXx2LXPsZ0zbhDigwVToQ9yL9G3BrX055qA8ZdM.2pKjwTTa_MnITc-mxMd8Thc8rg1Yye3uWkY41IOngi8&amp;dib_tag=se&amp;keywords=RTX+4090+Ti&amp;qid=1741743897&amp;sr=8-3</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>2025-03-11</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>ASUS ROG Herculx - Soporte antidesgarro para tarjeta gráfica (construcción de aleación de zinc maciza, fácil instalación sin herramientas, nivel de burbuja incluido, altura ajustable, amplia</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>Página 1 de 1</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>https://m.media-amazon.com/images/I/71m4QHLRzmL.__AC_SX300_SY300_QL70_ML2_.jpg</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com/-/es/ASUS-ROG-Herculx-antidesgarro-construcci%C3%B3n/dp/B0B173F6RM/ref=sr_1_4?dib=eyJ2IjoiMSJ9.Sv4Tuv8E6sKBPCb3XoqbMVCKzyZMgVXH7YU1musRODLJFBXGrEv9WxoP-U667nNFme06I0FFm3k7Exv4qh0zQBoDXzuBk4ciQo-2z40Rtc9lWWDggXK5PjgXdQesu8XaxZBtZSq5jbVf1SlVMK1wiWDwpWRz-5xXxgc5Ba9UMKm2e2eoYxiamKujSp1LfbSm__G3KXx2LXPsZ0zbhDigwVToQ9yL9G3BrX055qA8ZdM.2pKjwTTa_MnITc-mxMd8Thc8rg1Yye3uWkY41IOngi8&amp;dib_tag=se&amp;keywords=RTX+4090+Ti&amp;qid=1741743897&amp;sr=8-4</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>2025-03-11</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>Zotac Gaming RTX4060 Ti Twin Edge OC 8GB</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Página 1 de 1  </t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>https://m.media-amazon.com/images/I/61ss5pbQjQL.__AC_SY300_SX300_QL70_ML2_.jpg</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com/-/es/Zotac-Gaming-RTX4060-Twin-Edge/dp/B0C7178S9K/ref=sr_1_5?dib=eyJ2IjoiMSJ9.Sv4Tuv8E6sKBPCb3XoqbMVCKzyZMgVXH7YU1musRODLJFBXGrEv9WxoP-U667nNFme06I0FFm3k7Exv4qh0zQBoDXzuBk4ciQo-2z40Rtc9lWWDggXK5PjgXdQesu8XaxZBtZSq5jbVf1SlVMK1wiWDwpWRz-5xXxgc5Ba9UMKm2e2eoYxiamKujSp1LfbSm__G3KXx2LXPsZ0zbhDigwVToQ9yL9G3BrX055qA8ZdM.2pKjwTTa_MnITc-mxMd8Thc8rg1Yye3uWkY41IOngi8&amp;dib_tag=se&amp;keywords=RTX+4090+Ti&amp;qid=1741743897&amp;sr=8-5</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>2025-03-11</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>EVGA GeForce RTX 3070 Ti XC3 Ultra Gaming, 08G-P5-3785-KL, 8GB GDDR6X, refrigeración iCX3, ARGB LED, placa trasera de metal</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>https://m.media-amazon.com/images/I/615CYrZfwkS.__AC_SY300_SX300_QL70_ML2_.jpg</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com/-/es/GeForce-Gaming-08G-P5-3785-KL-refrigeraci%C3%B3n-trasera/dp/B097Z8YWW1/ref=sr_1_6?dib=eyJ2IjoiMSJ9.Sv4Tuv8E6sKBPCb3XoqbMVCKzyZMgVXH7YU1musRODLJFBXGrEv9WxoP-U667nNFme06I0FFm3k7Exv4qh0zQBoDXzuBk4ciQo-2z40Rtc9lWWDggXK5PjgXdQesu8XaxZBtZSq5jbVf1SlVMK1wiWDwpWRz-5xXxgc5Ba9UMKm2e2eoYxiamKujSp1LfbSm__G3KXx2LXPsZ0zbhDigwVToQ9yL9G3BrX055qA8ZdM.2pKjwTTa_MnITc-mxMd8Thc8rg1Yye3uWkY41IOngi8&amp;dib_tag=se&amp;keywords=RTX+4090+Ti&amp;qid=1741743897&amp;sr=8-6</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>2025-03-11</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>ZOTAC Gaming GeForce RTX 4060 Ti 16GB AMP DLSS 3 16GB GDDR6 128-bit 18 Gbps PCIE 4.0 Tarjeta gráfica compacta para juegos, refrigeración avanzada IceStorm 2.0, iluminación Spectra RGB, ZT-D40620F-10M</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Página 1 de 1  </t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>https://m.media-amazon.com/images/I/8153eBeVpQL.__AC_SY300_SX300_QL70_ML2_.jpg</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com/-/es/compacta-refrigeraci%C3%B3n-avanzada-iluminaci%C3%B3n-ZT-D40620F-10M/dp/B0CMJQZQC6/ref=sr_1_7?dib=eyJ2IjoiMSJ9.Sv4Tuv8E6sKBPCb3XoqbMVCKzyZMgVXH7YU1musRODLJFBXGrEv9WxoP-U667nNFme06I0FFm3k7Exv4qh0zQBoDXzuBk4ciQo-2z40Rtc9lWWDggXK5PjgXdQesu8XaxZBtZSq5jbVf1SlVMK1wiWDwpWRz-5xXxgc5Ba9UMKm2e2eoYxiamKujSp1LfbSm__G3KXx2LXPsZ0zbhDigwVToQ9yL9G3BrX055qA8ZdM.2pKjwTTa_MnITc-mxMd8Thc8rg1Yye3uWkY41IOngi8&amp;dib_tag=se&amp;keywords=RTX+4090+Ti&amp;qid=1741743897&amp;sr=8-7</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>2025-03-11</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>MSI Tarjeta gráfica Gaming RTX 4070 Ti Super 16G AERO (NVIDIA RTX 4070 Ti Super, 256-Bit, Boost Clock: 2610 MHz, 16GB GDRR6X 21 Gbps, HDMI/DP, Arquitectura Ada Lovelace)</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Página 1 de 1  </t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>https://m.media-amazon.com/images/I/61J3fQj9mgL.__AC_SY300_SX300_QL70_ML2_.jpg</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com/-/es/Tarjeta-gr%C3%A1fica-Gaming-NVIDIA-256-Bit/dp/B0CWS78Y5J/ref=sr_1_8?dib=eyJ2IjoiMSJ9.Sv4Tuv8E6sKBPCb3XoqbMVCKzyZMgVXH7YU1musRODLJFBXGrEv9WxoP-U667nNFme06I0FFm3k7Exv4qh0zQBoDXzuBk4ciQo-2z40Rtc9lWWDggXK5PjgXdQesu8XaxZBtZSq5jbVf1SlVMK1wiWDwpWRz-5xXxgc5Ba9UMKm2e2eoYxiamKujSp1LfbSm__G3KXx2LXPsZ0zbhDigwVToQ9yL9G3BrX055qA8ZdM.2pKjwTTa_MnITc-mxMd8Thc8rg1Yye3uWkY41IOngi8&amp;dib_tag=se&amp;keywords=RTX+4090+Ti&amp;qid=1741743897&amp;sr=8-8</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>2025-03-11</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>MSI Gaming GeForce RTX 4060 8GB GDRR6 Extreme Clock: 2505 MHz 128-Bit HDMI/DP Nvlink TORX Fan 4.0 Ada Lovelace Architecture Tarjeta gráfica (RTX 4060 Ventus 2X Blanco 8G OC)</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Página 1 de 1  </t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>https://m.media-amazon.com/images/I/71UcbpPyPLL.__AC_SY300_SX300_QL70_ML2_.jpg</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com/-/es/Gaming-GeForce-RTX-4060-Extreme/dp/B0CHC2LQF5/ref=sr_1_9?dib=eyJ2IjoiMSJ9.Sv4Tuv8E6sKBPCb3XoqbMVCKzyZMgVXH7YU1musRODLJFBXGrEv9WxoP-U667nNFme06I0FFm3k7Exv4qh0zQBoDXzuBk4ciQo-2z40Rtc9lWWDggXK5PjgXdQesu8XaxZBtZSq5jbVf1SlVMK1wiWDwpWRz-5xXxgc5Ba9UMKm2e2eoYxiamKujSp1LfbSm__G3KXx2LXPsZ0zbhDigwVToQ9yL9G3BrX055qA8ZdM.2pKjwTTa_MnITc-mxMd8Thc8rg1Yye3uWkY41IOngi8&amp;dib_tag=se&amp;keywords=RTX+4090+Ti&amp;qid=1741743897&amp;sr=8-9</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>2025-03-11</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>Tarjeta gráfica ProArt GeForce RTX™ 4070 Ti de 12 GB GDDR6X (PCIe 4.0, 12GB GDDR6X, DLSS 3, HDMI 2.1a, DisplayPort 1.4a)</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>Página 1 de 1</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>https://m.media-amazon.com/images/I/71CdtG8sQmL.__AC_SX300_SY300_QL70_ML2_.jpg</t>
+        </is>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com/-/es/Tarjeta-gr%C3%A1fica-ProArt-GeForce-DisplayPort/dp/B0C6FXM199/ref=sr_1_10?dib=eyJ2IjoiMSJ9.Sv4Tuv8E6sKBPCb3XoqbMVCKzyZMgVXH7YU1musRODLJFBXGrEv9WxoP-U667nNFme06I0FFm3k7Exv4qh0zQBoDXzuBk4ciQo-2z40Rtc9lWWDggXK5PjgXdQesu8XaxZBtZSq5jbVf1SlVMK1wiWDwpWRz-5xXxgc5Ba9UMKm2e2eoYxiamKujSp1LfbSm__G3KXx2LXPsZ0zbhDigwVToQ9yL9G3BrX055qA8ZdM.2pKjwTTa_MnITc-mxMd8Thc8rg1Yye3uWkY41IOngi8&amp;dib_tag=se&amp;keywords=RTX+4090+Ti&amp;qid=1741743897&amp;sr=8-10</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>2025-03-11</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>SAMSUNG Galaxy Z Flip 6 AI - Teléfono celular, 256 GB desbloqueado, teléfono inteligente Android desbloqueado, FlexCam, asistente de fotos, modo videocámara, intérprete en vivo, diseño plegable, 2024,</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>US$949.99</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>https://m.media-amazon.com/images/I/61I57TD66QL.__AC_SX300_SY300_QL70_ML2_.jpg</t>
+        </is>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com/-/es/sspa/click?ie=UTF8&amp;spc=MTozNTMzNzg3MDA3NTU0NzM3OjE3NDE3NDQwOTY6c3BfYXRmOjMwMDQ1NTcwOTA0MTUwMjo6MDo6&amp;url=%2FSAMSUNG-Galaxy-Flip-desbloqueado-inteligente%2Fdp%2FB0D191BM26%2Fref%3Dsr_1_1_sspa%3Fdib%3DeyJ2IjoiMSJ9.Vr9gE1FAeve6BjH2AGvo9M-qkfQRX2q1gWyBHO1W4tCp65ABpKeSjNka16Fqp_t_ic6XFI34IpB3RrgFcPxiJQ0JuCmQ1xdvvOcMbc_MzJJ_kUMgMI8c2AoBq0Go0U9WQxMNn9k8IFm9n8xuMGThRDkHDOWQ1B5RPfeAWLULyr5j1O5RPuxPKpnh_I3wYMZ1k09XViTQsEB_eF8Tp-oNEtaBCiSSSomvqTABTDYeYaU.IDwD49sayJDppcHVXZ3tlG6zhq1RCl0sp5QnkzAe4f8%26dib_tag%3Dse%26keywords%3DSAMSUNG%2BGALAXY%2BS25%2BULTRA%26qid%3D1741744096%26sr%3D8-1-spons%26sp_csd%3Dd2lkZ2V0TmFtZT1zcF9hdGY%26psc%3D1</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>2025-03-11</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>Teléfono I24 Ultra, teléfono desbloqueado de 8+256 GB, teléfono inteligente Android 13, cámara de 48+108MP, bolígrafo integrado, batería de 6800 mAh, SIM dual, pantalla HD de 6.8 pulgadas,</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>US$179.99</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>https://m.media-amazon.com/images/I/81gKQc9moRL.__AC_SX300_SY300_QL70_ML2_.jpg</t>
+        </is>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com/-/es/sspa/click?ie=UTF8&amp;spc=MTozNTMzNzg3MDA3NTU0NzM3OjE3NDE3NDQwOTY6c3BfYXRmOjMwMDY2MzY3NTE5NTYwMjo6MDo6&amp;url=%2FI24-Ultra-desbloqueado-inteligente-bol%25C3%25ADgrafo%2Fdp%2FB0DSW8RPQM%2Fref%3Dsr_1_2_sspa%3Fdib%3DeyJ2IjoiMSJ9.Vr9gE1FAeve6BjH2AGvo9M-qkfQRX2q1gWyBHO1W4tCp65ABpKeSjNka16Fqp_t_ic6XFI34IpB3RrgFcPxiJQ0JuCmQ1xdvvOcMbc_MzJJ_kUMgMI8c2AoBq0Go0U9WQxMNn9k8IFm9n8xuMGThRDkHDOWQ1B5RPfeAWLULyr5j1O5RPuxPKpnh_I3wYMZ1k09XViTQsEB_eF8Tp-oNEtaBCiSSSomvqTABTDYeYaU.IDwD49sayJDppcHVXZ3tlG6zhq1RCl0sp5QnkzAe4f8%26dib_tag%3Dse%26keywords%3DSAMSUNG%2BGALAXY%2BS25%2BULTRA%26qid%3D1741744096%26sr%3D8-2-spons%26sp_csd%3Dd2lkZ2V0TmFtZT1zcF9hdGY%26psc%3D1</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>2025-03-11</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>SAMSUNG Galaxy S24 Ultra SM-S928B/DS 12GB 256GB Dual Sim Modelo Internacional Desbloqueado de Fábrica (gris titanio)</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>US$905.00</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>https://m.media-amazon.com/images/I/51EldjH4K8L.__AC_SX300_SY300_QL70_ML2_.jpg</t>
+        </is>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com/-/es/SAMSUNG-SM-S928B-Internacional-Desbloqueado-F%C3%A1brica/dp/B0CT45DH2H/ref=sr_1_3?dib=eyJ2IjoiMSJ9.Vr9gE1FAeve6BjH2AGvo9M-qkfQRX2q1gWyBHO1W4tCp65ABpKeSjNka16Fqp_t_ic6XFI34IpB3RrgFcPxiJQ0JuCmQ1xdvvOcMbc_MzJJ_kUMgMI8c2AoBq0Go0U9WQxMNn9k8IFm9n8xuMGThRDkHDOWQ1B5RPfeAWLULyr5j1O5RPuxPKpnh_I3wYMZ1k09XViTQsEB_eF8Tp-oNEtaBCiSSSomvqTABTDYeYaU.IDwD49sayJDppcHVXZ3tlG6zhq1RCl0sp5QnkzAe4f8&amp;dib_tag=se&amp;keywords=SAMSUNG+GALAXY+S25+ULTRA&amp;qid=1741744096&amp;sr=8-3</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>2025-03-11</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>SAMSUNG Teléfono Galaxy S24 FE AI, teléfono inteligente Android desbloqueado de 128 GB, cámara de alta resolución de 50 MP, batería de larga duración, pantalla de visualización más brillante, versión</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>US$498.95</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>https://m.media-amazon.com/images/I/61uakkLoHxL.__AC_SX300_SY300_QL70_ML2_.jpg</t>
+        </is>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com/-/es/inteligente-desbloqueado-resoluci%C3%B3n-visualizaci%C3%B3n-brillante/dp/B0DCLCPN9T/ref=sr_1_4?dib=eyJ2IjoiMSJ9.Vr9gE1FAeve6BjH2AGvo9M-qkfQRX2q1gWyBHO1W4tCp65ABpKeSjNka16Fqp_t_ic6XFI34IpB3RrgFcPxiJQ0JuCmQ1xdvvOcMbc_MzJJ_kUMgMI8c2AoBq0Go0U9WQxMNn9k8IFm9n8xuMGThRDkHDOWQ1B5RPfeAWLULyr5j1O5RPuxPKpnh_I3wYMZ1k09XViTQsEB_eF8Tp-oNEtaBCiSSSomvqTABTDYeYaU.IDwD49sayJDppcHVXZ3tlG6zhq1RCl0sp5QnkzAe4f8&amp;dib_tag=se&amp;keywords=SAMSUNG+GALAXY+S25+ULTRA&amp;qid=1741744096&amp;sr=8-4</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>2025-03-11</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>SAMSUNG Teléfono celular Galaxy S24 Ultra, teléfono inteligente AI de 256 GB, Android desbloqueado, 200 MP, cámaras zoom 100x, batería de larga duración, S Pen, versión global, 2024 - negro titanio</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>US$910.00</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>https://m.media-amazon.com/images/I/51MZ3NnjXUL.__AC_SX300_SY300_QL70_ML2_.jpg</t>
+        </is>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com/-/es/Tel%C3%A9fono-tel%C3%A9fono-inteligente-desbloqueado-duraci%C3%B3n/dp/B0D51S487S/ref=sr_1_5?dib=eyJ2IjoiMSJ9.Vr9gE1FAeve6BjH2AGvo9M-qkfQRX2q1gWyBHO1W4tCp65ABpKeSjNka16Fqp_t_ic6XFI34IpB3RrgFcPxiJQ0JuCmQ1xdvvOcMbc_MzJJ_kUMgMI8c2AoBq0Go0U9WQxMNn9k8IFm9n8xuMGThRDkHDOWQ1B5RPfeAWLULyr5j1O5RPuxPKpnh_I3wYMZ1k09XViTQsEB_eF8Tp-oNEtaBCiSSSomvqTABTDYeYaU.IDwD49sayJDppcHVXZ3tlG6zhq1RCl0sp5QnkzAe4f8&amp;dib_tag=se&amp;keywords=SAMSUNG+GALAXY+S25+ULTRA&amp;qid=1741744096&amp;sr=8-5</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>2025-03-11</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>SAMSUNG Teléfono celular Galaxy S25, teléfono inteligente AI de 128 GB, Android desbloqueado, cámara AI, procesador rápido, pantalla ProScaler, batería de larga duración, 2025, Icyblue</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>US$719.99</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>https://m.media-amazon.com/images/I/61LAKVCKRvL.__AC_SX300_SY300_QL70_ML2_.jpg</t>
+        </is>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com/-/es/Tel%C3%A9fono-inteligente-desbloqueado-procesador-ProScaler/dp/B0DP3DB4CW/ref=sr_1_6?dib=eyJ2IjoiMSJ9.Vr9gE1FAeve6BjH2AGvo9M-qkfQRX2q1gWyBHO1W4tCp65ABpKeSjNka16Fqp_t_ic6XFI34IpB3RrgFcPxiJQ0JuCmQ1xdvvOcMbc_MzJJ_kUMgMI8c2AoBq0Go0U9WQxMNn9k8IFm9n8xuMGThRDkHDOWQ1B5RPfeAWLULyr5j1O5RPuxPKpnh_I3wYMZ1k09XViTQsEB_eF8Tp-oNEtaBCiSSSomvqTABTDYeYaU.IDwD49sayJDppcHVXZ3tlG6zhq1RCl0sp5QnkzAe4f8&amp;dib_tag=se&amp;keywords=SAMSUNG+GALAXY+S25+ULTRA&amp;qid=1741744096&amp;sr=8-6</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>2025-03-11</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>Funda para Samsung Galaxy S25 Ultra con soporte magnético, compatible con MagSafe Ring Leather Case, con lente de cámara y protector de pantalla, protección de grado militar, a prueba de</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>US$26.99</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>https://m.media-amazon.com/images/I/71Z4J-Y20-L.__AC_SX300_SY300_QL70_ML2_.jpg</t>
+        </is>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com/-/es/sspa/click?ie=UTF8&amp;spc=MTozNTMzNzg3MDA3NTU0NzM3OjE3NDE3NDQwOTY6c3BfbXRmOjMwMDY1NDMxNTMxNDMwMjo6MDo6&amp;url=%2FBullroye-magn%25C3%25A9tico-compatible-protector-protecci%25C3%25B3n%2Fdp%2FB0DPM996GT%2Fref%3Dsr_1_7_sspa%3Fdib%3DeyJ2IjoiMSJ9.Vr9gE1FAeve6BjH2AGvo9M-qkfQRX2q1gWyBHO1W4tCp65ABpKeSjNka16Fqp_t_ic6XFI34IpB3RrgFcPxiJQ0JuCmQ1xdvvOcMbc_MzJJ_kUMgMI8c2AoBq0Go0U9WQxMNn9k8IFm9n8xuMGThRDkHDOWQ1B5RPfeAWLULyr5j1O5RPuxPKpnh_I3wYMZ1k09XViTQsEB_eF8Tp-oNEtaBCiSSSomvqTABTDYeYaU.IDwD49sayJDppcHVXZ3tlG6zhq1RCl0sp5QnkzAe4f8%26dib_tag%3Dse%26keywords%3DSAMSUNG%2BGALAXY%2BS25%2BULTRA%26qid%3D1741744096%26sr%3D8-7-spons%26sp_csd%3Dd2lkZ2V0TmFtZT1zcF9tdGY%26psc%3D1</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>2025-03-11</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>SAMSUNG Galaxy S24 Ultra 5G S9280 Physical Dual SIM 512GB 12GB RAM AI Smartphone, desbloqueado de fábrica, modelo global, batería de larga duración - Violeta titanio</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>https://m.media-amazon.com/images/I/418KI8X9QBL.__AC_SX300_SY300_QL70_ML2_.jpg</t>
+        </is>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com/-/es/S9280-Physical-Smartphone-desbloqueado-duraci%C3%B3n/dp/B0CV73SG4Z/ref=sr_1_8?dib=eyJ2IjoiMSJ9.Vr9gE1FAeve6BjH2AGvo9M-qkfQRX2q1gWyBHO1W4tCp65ABpKeSjNka16Fqp_t_ic6XFI34IpB3RrgFcPxiJQ0JuCmQ1xdvvOcMbc_MzJJ_kUMgMI8c2AoBq0Go0U9WQxMNn9k8IFm9n8xuMGThRDkHDOWQ1B5RPfeAWLULyr5j1O5RPuxPKpnh_I3wYMZ1k09XViTQsEB_eF8Tp-oNEtaBCiSSSomvqTABTDYeYaU.IDwD49sayJDppcHVXZ3tlG6zhq1RCl0sp5QnkzAe4f8&amp;dib_tag=se&amp;keywords=SAMSUNG+GALAXY+S25+ULTRA&amp;qid=1741744096&amp;sr=8-8</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>2025-03-11</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>Samsung Teléfono celular Galaxy S24 Ultra, teléfono inteligente AI de 256 GB, Android desbloqueado, 200 MP, cámaras zoom 100x, procesador rápido, batería de larga duración, pantalla de borde a borde,</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Página 1 de 1  </t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>https://m.media-amazon.com/images/I/71-EnPs+uQL._AC_SY300_SX300_.jpg</t>
+        </is>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com/-/es/Tel%C3%A9fono-tel%C3%A9fono-inteligente-desbloqueado-procesador/dp/B0CMDL3H3P/ref=sr_1_9?dib=eyJ2IjoiMSJ9.Vr9gE1FAeve6BjH2AGvo9M-qkfQRX2q1gWyBHO1W4tCp65ABpKeSjNka16Fqp_t_ic6XFI34IpB3RrgFcPxiJQ0JuCmQ1xdvvOcMbc_MzJJ_kUMgMI8c2AoBq0Go0U9WQxMNn9k8IFm9n8xuMGThRDkHDOWQ1B5RPfeAWLULyr5j1O5RPuxPKpnh_I3wYMZ1k09XViTQsEB_eF8Tp-oNEtaBCiSSSomvqTABTDYeYaU.IDwD49sayJDppcHVXZ3tlG6zhq1RCl0sp5QnkzAe4f8&amp;dib_tag=se&amp;keywords=SAMSUNG+GALAXY+S25+ULTRA&amp;qid=1741744096&amp;sr=8-9</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>2025-03-11</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>SAMSUNG Galaxy S24 Ultra Dual SIM SM-S928B/DS Dual Sim EU/UK Modelo 12GB Ram 256 GB Almacenamiento desbloqueado de fábrica (violeta titanio)</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>US$875.00</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>https://m.media-amazon.com/images/I/51A4DBUBcTL.__AC_SX300_SY300_QL70_ML2_.jpg</t>
+        </is>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com/-/es/SAMSUNG-SM-S928B-Almacenamiento-desbloqueado-f%C3%A1brica/dp/B0CT422655/ref=sr_1_10?dib=eyJ2IjoiMSJ9.Vr9gE1FAeve6BjH2AGvo9M-qkfQRX2q1gWyBHO1W4tCp65ABpKeSjNka16Fqp_t_ic6XFI34IpB3RrgFcPxiJQ0JuCmQ1xdvvOcMbc_MzJJ_kUMgMI8c2AoBq0Go0U9WQxMNn9k8IFm9n8xuMGThRDkHDOWQ1B5RPfeAWLULyr5j1O5RPuxPKpnh_I3wYMZ1k09XViTQsEB_eF8Tp-oNEtaBCiSSSomvqTABTDYeYaU.IDwD49sayJDppcHVXZ3tlG6zhq1RCl0sp5QnkzAe4f8&amp;dib_tag=se&amp;keywords=SAMSUNG+GALAXY+S25+ULTRA&amp;qid=1741744096&amp;sr=8-10</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>2025-03-11</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>Apple Watch Series 10 (46 mm, GPS) con caja de aluminio oro rosa, correa loop deportiva ciruela monitor fitness, app ECG, pantalla Retina siempre activa, neutro en carbono</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>No se encontró el precio del producto</t>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>https://m.media-amazon.com/images/I/81CPZEl9HyL.__AC_SY445_SX342_QL70_ML2_.jpg</t>
+        </is>
+      </c>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com/-/es/aluminio-deportiva-ciruela-monitor-pantalla/dp/B0DGHV2B2Z/ref=sr_1_1?dib=eyJ2IjoiMSJ9.c1pZhfCe88kb98mf9jarSXqHIUkW5kvj95Y3TEeBQTsshYer1fMaGWBgUi2vXEVRNsYwY8lA7vTdZQ-MZJbBzIoV67zTVlU6XmYZU3IMGmaXcIJ1iGjVJn_YswTazjnqAsn9TL4vH32XSjyMjIiDFiNVOvha0FkWR3uFevOMDVsQBT7rdTxReq28R5zST1UETBXf4BCJuLEPzGkuzehh5n17mWHp6rPgGStXuE2xSIU.7xd1rRh6bCmr7KP1mln16ldgmOlpwX-mMJSEIw8xBvc&amp;dib_tag=se&amp;keywords=Apple+watch&amp;qid=1741744541&amp;sr=8-1</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>2025-03-11</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>Apple Reloj Serie 5 (GPS, 1.575 pulgadas) - Caja de aluminio plateada con correa deportiva blanca (renovada)</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>US$124.99</t>
+        </is>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>https://m.media-amazon.com/images/I/71nbXdvdGfL.__AC_SX300_SY300_QL70_ML2_.jpg</t>
+        </is>
+      </c>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com/-/es/Apple-Reloj-Serie-1-575-pulgadas/dp/B0842BFWZV/ref=sr_1_2?dib=eyJ2IjoiMSJ9.c1pZhfCe88kb98mf9jarSXqHIUkW5kvj95Y3TEeBQTsshYer1fMaGWBgUi2vXEVRNsYwY8lA7vTdZQ-MZJbBzIoV67zTVlU6XmYZU3IMGmaXcIJ1iGjVJn_YswTazjnqAsn9TL4vH32XSjyMjIiDFiNVOvha0FkWR3uFevOMDVsQBT7rdTxReq28R5zST1UETBXf4BCJuLEPzGkuzehh5n17mWHp6rPgGStXuE2xSIU.7xd1rRh6bCmr7KP1mln16ldgmOlpwX-mMJSEIw8xBvc&amp;dib_tag=se&amp;keywords=Apple+watch&amp;qid=1741744541&amp;sr=8-2</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>2025-03-11</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>Apple Watch - Serie 7 con GPS + celular y caja de aluminio Starlight de 1.61 pulgadas (41mm) con correa deportiva Starlight, tamaño regular (renovado)</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>US$169.00</t>
+        </is>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>https://m.media-amazon.com/images/I/51478LBC2rL.__AC_SX300_SY300_QL70_ML2_.jpg</t>
+        </is>
+      </c>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com/-/es/Apple-Watch-aluminio-Starlight-deportiva/dp/B09NWHNN15/ref=sr_1_3?dib=eyJ2IjoiMSJ9.c1pZhfCe88kb98mf9jarSXqHIUkW5kvj95Y3TEeBQTsshYer1fMaGWBgUi2vXEVRNsYwY8lA7vTdZQ-MZJbBzIoV67zTVlU6XmYZU3IMGmaXcIJ1iGjVJn_YswTazjnqAsn9TL4vH32XSjyMjIiDFiNVOvha0FkWR3uFevOMDVsQBT7rdTxReq28R5zST1UETBXf4BCJuLEPzGkuzehh5n17mWHp6rPgGStXuE2xSIU.7xd1rRh6bCmr7KP1mln16ldgmOlpwX-mMJSEIw8xBvc&amp;dib_tag=se&amp;keywords=Apple+watch&amp;qid=1741744541&amp;sr=8-3</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>2025-03-11</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>Apple iPad Air, 10.9 pulgadas, con wifi, 64 GB, azul cielo, 4.ª generación, renovado.</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>US$148.00</t>
+        </is>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>https://m.media-amazon.com/images/I/71aLryIN+ZL._AC_SY300_SX300_.jpg</t>
+        </is>
+      </c>
+      <c r="E55" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com/-/es/Apple-pulgadas-cielo-generaci%C3%B3n-renovado/dp/B08KGVJQC8/ref=sr_1_4?dib=eyJ2IjoiMSJ9.c1pZhfCe88kb98mf9jarSXqHIUkW5kvj95Y3TEeBQTsshYer1fMaGWBgUi2vXEVRNsYwY8lA7vTdZQ-MZJbBzIoV67zTVlU6XmYZU3IMGmaXcIJ1iGjVJn_YswTazjnqAsn9TL4vH32XSjyMjIiDFiNVOvha0FkWR3uFevOMDVsQBT7rdTxReq28R5zST1UETBXf4BCJuLEPzGkuzehh5n17mWHp6rPgGStXuE2xSIU.7xd1rRh6bCmr7KP1mln16ldgmOlpwX-mMJSEIw8xBvc&amp;dib_tag=se&amp;keywords=Apple+watch&amp;qid=1741744541&amp;sr=8-4</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>2025-03-11</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>Apple iPad Air, 10.9 pulgadas, con wifi, 64 GB, azul cielo, 4.ª generación, renovado.</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>US$148.00</t>
+        </is>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>https://m.media-amazon.com/images/I/71K+hTswAyL._AC_SY300_SX300_.jpg</t>
+        </is>
+      </c>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com/-/es/Apple-pulgadas-cielo-generaci%C3%B3n-renovado/dp/B08KZYMNJC/ref=sr_1_5?dib=eyJ2IjoiMSJ9.c1pZhfCe88kb98mf9jarSXqHIUkW5kvj95Y3TEeBQTsshYer1fMaGWBgUi2vXEVRNsYwY8lA7vTdZQ-MZJbBzIoV67zTVlU6XmYZU3IMGmaXcIJ1iGjVJn_YswTazjnqAsn9TL4vH32XSjyMjIiDFiNVOvha0FkWR3uFevOMDVsQBT7rdTxReq28R5zST1UETBXf4BCJuLEPzGkuzehh5n17mWHp6rPgGStXuE2xSIU.7xd1rRh6bCmr7KP1mln16ldgmOlpwX-mMJSEIw8xBvc&amp;dib_tag=se&amp;keywords=Apple+watch&amp;qid=1741744541&amp;sr=8-5</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>2025-03-11</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>Apple Watch Series 8 - Reloj inteligente con caja de aluminio de color negro (Midnight) y correa deportiva de color negro (Midnight), M/L (renovado) (GPS, 45 mm)</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>US$214.00</t>
+        </is>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>https://m.media-amazon.com/images/I/71XMTLtZd5L.__AC_SX300_SY300_QL70_ML2_.jpg</t>
+        </is>
+      </c>
+      <c r="E57" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com/-/es/Apple-Watch-inteligente-aluminio-deportiva/dp/B0BS4D5C8D/ref=sr_1_6?dib=eyJ2IjoiMSJ9.c1pZhfCe88kb98mf9jarSXqHIUkW5kvj95Y3TEeBQTsshYer1fMaGWBgUi2vXEVRNsYwY8lA7vTdZQ-MZJbBzIoV67zTVlU6XmYZU3IMGmaXcIJ1iGjVJn_YswTazjnqAsn9TL4vH32XSjyMjIiDFiNVOvha0FkWR3uFevOMDVsQBT7rdTxReq28R5zST1UETBXf4BCJuLEPzGkuzehh5n17mWHp6rPgGStXuE2xSIU.7xd1rRh6bCmr7KP1mln16ldgmOlpwX-mMJSEIw8xBvc&amp;dib_tag=se&amp;keywords=Apple+watch&amp;qid=1741744541&amp;sr=8-6</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>2025-03-11</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>Apple Reloj inteligente de la serie 9 [GPS + celular de 1.614 in] con caja de aluminio rosa con correa deportiva rosa S/M. Monitor de fitness, aplicaciones de oxígeno en sangre y ECG, pantalla de</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>US$252.69</t>
+        </is>
+      </c>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>https://m.media-amazon.com/images/I/61AgWAxKnlL.__AC_SX300_SY300_QL70_ML2_.jpg</t>
+        </is>
+      </c>
+      <c r="E58" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com/-/es/inteligente-aluminio-deportiva-aplicaciones-pantalla/dp/B0CTD9PNT2/ref=sr_1_7?dib=eyJ2IjoiMSJ9.c1pZhfCe88kb98mf9jarSXqHIUkW5kvj95Y3TEeBQTsshYer1fMaGWBgUi2vXEVRNsYwY8lA7vTdZQ-MZJbBzIoV67zTVlU6XmYZU3IMGmaXcIJ1iGjVJn_YswTazjnqAsn9TL4vH32XSjyMjIiDFiNVOvha0FkWR3uFevOMDVsQBT7rdTxReq28R5zST1UETBXf4BCJuLEPzGkuzehh5n17mWHp6rPgGStXuE2xSIU.7xd1rRh6bCmr7KP1mln16ldgmOlpwX-mMJSEIw8xBvc&amp;dib_tag=se&amp;keywords=Apple+watch&amp;qid=1741744541&amp;sr=8-7</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>2025-03-11</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>Apple Watch - Serie 7 con GPS y caja de aluminio color azul oscuro de 1.77 pulgadas (45mm) con correa deportiva color azul oscuro, tamaño regular (renovado)</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>US$169.00</t>
+        </is>
+      </c>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>https://m.media-amazon.com/images/I/51I1QoWjX3L.__AC_SX300_SY300_QL70_ML2_.jpg</t>
+        </is>
+      </c>
+      <c r="E59" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com/-/es/Apple-Watch-aluminio-pulgadas-deportiva/dp/B09NWDXS13/ref=sr_1_8?dib=eyJ2IjoiMSJ9.c1pZhfCe88kb98mf9jarSXqHIUkW5kvj95Y3TEeBQTsshYer1fMaGWBgUi2vXEVRNsYwY8lA7vTdZQ-MZJbBzIoV67zTVlU6XmYZU3IMGmaXcIJ1iGjVJn_YswTazjnqAsn9TL4vH32XSjyMjIiDFiNVOvha0FkWR3uFevOMDVsQBT7rdTxReq28R5zST1UETBXf4BCJuLEPzGkuzehh5n17mWHp6rPgGStXuE2xSIU.7xd1rRh6bCmr7KP1mln16ldgmOlpwX-mMJSEIw8xBvc&amp;dib_tag=se&amp;keywords=Apple+watch&amp;qid=1741744541&amp;sr=8-8</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>2025-03-11</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>Apple iPad Air, 10.9 pulgadas, con wifi, 64 GB, azul cielo, 4.ª generación, renovado</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>US$139.00</t>
+        </is>
+      </c>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t>https://m.media-amazon.com/images/I/51rQ99P6djL.__AC_SX300_SY300_QL70_ML2_.jpg</t>
+        </is>
+      </c>
+      <c r="E60" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com/-/es/Apple-pulgadas-cielo-generaci%C3%B3n-renovado/dp/B08KYJPTB6/ref=sr_1_9?dib=eyJ2IjoiMSJ9.c1pZhfCe88kb98mf9jarSXqHIUkW5kvj95Y3TEeBQTsshYer1fMaGWBgUi2vXEVRNsYwY8lA7vTdZQ-MZJbBzIoV67zTVlU6XmYZU3IMGmaXcIJ1iGjVJn_YswTazjnqAsn9TL4vH32XSjyMjIiDFiNVOvha0FkWR3uFevOMDVsQBT7rdTxReq28R5zST1UETBXf4BCJuLEPzGkuzehh5n17mWHp6rPgGStXuE2xSIU.7xd1rRh6bCmr7KP1mln16ldgmOlpwX-mMJSEIw8xBvc&amp;dib_tag=se&amp;keywords=Apple+watch&amp;qid=1741744541&amp;sr=8-9</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>2025-03-11</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>Apple Reloj SE (2.ª generación) (GPS, 1.575 pulgadas) - Caja de aluminio Starlight con correa deportiva Starlight, S/M (renovado)</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>US$169.99</t>
+        </is>
+      </c>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t>https://m.media-amazon.com/images/I/71YdE55GwjL.__AC_SX300_SY300_QL70_ML2_.jpg</t>
+        </is>
+      </c>
+      <c r="E61" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com/-/es/Apple-Reloj-generaci%C3%B3n-1-575-pulgadas/dp/B0BWPK91TB/ref=sr_1_10?dib=eyJ2IjoiMSJ9.c1pZhfCe88kb98mf9jarSXqHIUkW5kvj95Y3TEeBQTsshYer1fMaGWBgUi2vXEVRNsYwY8lA7vTdZQ-MZJbBzIoV67zTVlU6XmYZU3IMGmaXcIJ1iGjVJn_YswTazjnqAsn9TL4vH32XSjyMjIiDFiNVOvha0FkWR3uFevOMDVsQBT7rdTxReq28R5zST1UETBXf4BCJuLEPzGkuzehh5n17mWHp6rPgGStXuE2xSIU.7xd1rRh6bCmr7KP1mln16ldgmOlpwX-mMJSEIw8xBvc&amp;dib_tag=se&amp;keywords=Apple+watch&amp;qid=1741744541&amp;sr=8-10</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>2025-03-11</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>Intel® CoreTM i9-14900K Nuevo procesador de escritorio para juegos 24 (8 núcleos P + 16 núcleos E) con gráficos integrados - Desbloqueado</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>US$445.00</t>
+        </is>
+      </c>
+      <c r="D62" t="inlineStr">
+        <is>
+          <t>https://m.media-amazon.com/images/I/51kMh915XHL.__AC_SX300_SY300_QL70_ML2_.jpg</t>
+        </is>
+      </c>
+      <c r="E62" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com/-/es/i9-14900K-procesador-escritorio-gr%C3%A1ficos-integrados/dp/B0CGJDKLB8/ref=sr_1_1?dib=eyJ2IjoiMSJ9.P2PLhYPu7OgM1kXe615j_13E_oDbE9Lu4hclIVsh8DkmIMWX2-yhMxf0e-LEicdCjc_e8VaSdFGU5LE--gLEwC2sH71I3ilJEfJpwvfAPzgIh04UBiFVW5YLSo1Yy9chFDQbvV13HT5SUyWl0hRRShtLRX1_aevA4aWrs5hyEj3jNtJ3Mc3G3UMqujfda3kl2tuo-XMZ-H0AtccGyohL5yg5Sgp7uLpaxlWpWoUwLJw.BwmGUQgnLk4bZfTX15D7Ltvw2Iz-akDh1ZogKg3HGPg&amp;dib_tag=se&amp;keywords=Intel+core+i9+14900K&amp;qid=1741745328&amp;sr=8-1</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>2025-03-11</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>Intel® Procesador de escritorio Core™ i9-14900K 24 núcleos (8 núcleos P + 16 núcleos E) hasta 6.0 GHz</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>US$445.00</t>
+        </is>
+      </c>
+      <c r="D63" t="inlineStr">
+        <is>
+          <t>https://m.media-amazon.com/images/I/61a+cNGLTvL._AC_SY300_SX300_.jpg</t>
+        </is>
+      </c>
+      <c r="E63" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com/-/es/Intel%C2%AE-Procesador-escritorio-i9-14900K-n%C3%BAcleos/dp/B0CHBJGFBC/ref=sr_1_2?dib=eyJ2IjoiMSJ9.P2PLhYPu7OgM1kXe615j_13E_oDbE9Lu4hclIVsh8DkmIMWX2-yhMxf0e-LEicdCjc_e8VaSdFGU5LE--gLEwC2sH71I3ilJEfJpwvfAPzgIh04UBiFVW5YLSo1Yy9chFDQbvV13HT5SUyWl0hRRShtLRX1_aevA4aWrs5hyEj3jNtJ3Mc3G3UMqujfda3kl2tuo-XMZ-H0AtccGyohL5yg5Sgp7uLpaxlWpWoUwLJw.BwmGUQgnLk4bZfTX15D7Ltvw2Iz-akDh1ZogKg3HGPg&amp;dib_tag=se&amp;keywords=Intel+core+i9+14900K&amp;qid=1741745328&amp;sr=8-2</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>2025-03-11</t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>Intel® Procesador de escritorio Core™ i9-14900KS 24 núcleos (8 núcleos P + 16 núcleos E)</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>US$669.99</t>
+        </is>
+      </c>
+      <c r="D64" t="inlineStr">
+        <is>
+          <t>https://m.media-amazon.com/images/I/51KxsgP0HlL.__AC_SX300_SY300_QL70_ML2_.jpg</t>
+        </is>
+      </c>
+      <c r="E64" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com/-/es/Intel%C2%AE-Procesador-escritorio-i9-14900KS-n%C3%BAcleos/dp/B0CXHMTHWP/ref=sr_1_3?dib=eyJ2IjoiMSJ9.P2PLhYPu7OgM1kXe615j_13E_oDbE9Lu4hclIVsh8DkmIMWX2-yhMxf0e-LEicdCjc_e8VaSdFGU5LE--gLEwC2sH71I3ilJEfJpwvfAPzgIh04UBiFVW5YLSo1Yy9chFDQbvV13HT5SUyWl0hRRShtLRX1_aevA4aWrs5hyEj3jNtJ3Mc3G3UMqujfda3kl2tuo-XMZ-H0AtccGyohL5yg5Sgp7uLpaxlWpWoUwLJw.BwmGUQgnLk4bZfTX15D7Ltvw2Iz-akDh1ZogKg3HGPg&amp;dib_tag=se&amp;keywords=Intel+core+i9+14900K&amp;qid=1741745328&amp;sr=8-3</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>2025-03-11</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>Intel Procesador de escritorio Core Ultra 9 285K - 24 núcleos (8 núcleos P + 16 núcleos E) hasta 5.7 GHz</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>US$619.99</t>
+        </is>
+      </c>
+      <c r="D65" t="inlineStr">
+        <is>
+          <t>https://m.media-amazon.com/images/I/51xxm7JkJ6L.__AC_SX300_SY300_QL70_ML2_.jpg</t>
+        </is>
+      </c>
+      <c r="E65" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com/-/es/Intel-Procesador-Core-Ultra-285K/dp/B0DFKC99VL/ref=sr_1_4?dib=eyJ2IjoiMSJ9.P2PLhYPu7OgM1kXe615j_13E_oDbE9Lu4hclIVsh8DkmIMWX2-yhMxf0e-LEicdCjc_e8VaSdFGU5LE--gLEwC2sH71I3ilJEfJpwvfAPzgIh04UBiFVW5YLSo1Yy9chFDQbvV13HT5SUyWl0hRRShtLRX1_aevA4aWrs5hyEj3jNtJ3Mc3G3UMqujfda3kl2tuo-XMZ-H0AtccGyohL5yg5Sgp7uLpaxlWpWoUwLJw.BwmGUQgnLk4bZfTX15D7Ltvw2Iz-akDh1ZogKg3HGPg&amp;dib_tag=se&amp;keywords=Intel+core+i9+14900K&amp;qid=1741745328&amp;sr=8-4</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>2025-03-11</t>
+        </is>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>Intel Core i9-12900K Procesador de escritorio para juegos con gráficos integrados y 16 núcleos (8P+8E) hasta 5.2 GHz desbloqueado LGA1700 Serie 600 Chipset 125W</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>US$323.19</t>
+        </is>
+      </c>
+      <c r="D66" t="inlineStr">
+        <is>
+          <t>https://m.media-amazon.com/images/I/51klBAsxGHL.__AC_SX300_SY300_QL70_ML2_.jpg</t>
+        </is>
+      </c>
+      <c r="E66" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com/-/es/i9-12900K-Procesador-escritorio-integrados-desbloqueado/dp/B09FXDLX95/ref=sr_1_5?dib=eyJ2IjoiMSJ9.P2PLhYPu7OgM1kXe615j_13E_oDbE9Lu4hclIVsh8DkmIMWX2-yhMxf0e-LEicdCjc_e8VaSdFGU5LE--gLEwC2sH71I3ilJEfJpwvfAPzgIh04UBiFVW5YLSo1Yy9chFDQbvV13HT5SUyWl0hRRShtLRX1_aevA4aWrs5hyEj3jNtJ3Mc3G3UMqujfda3kl2tuo-XMZ-H0AtccGyohL5yg5Sgp7uLpaxlWpWoUwLJw.BwmGUQgnLk4bZfTX15D7Ltvw2Iz-akDh1ZogKg3HGPg&amp;dib_tag=se&amp;keywords=Intel+core+i9+14900K&amp;qid=1741745328&amp;sr=8-5</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>2025-03-11</t>
+        </is>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>Intel Core i9-12900KF Procesador de escritorio para juegos 16 (8P+8E) núcleos hasta 5.2 GHz desbloqueado LGA1700 Serie 600 Chipset 125W</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>US$299.00</t>
+        </is>
+      </c>
+      <c r="D67" t="inlineStr">
+        <is>
+          <t>https://m.media-amazon.com/images/I/51CUAct4KVL.__AC_SX300_SY300_QL70_ML2_.jpg</t>
+        </is>
+      </c>
+      <c r="E67" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com/-/es/i9-12900KF-Procesador-escritorio-n%C3%BAcleos-desbloqueado/dp/B09FWYK5M9/ref=sr_1_6?dib=eyJ2IjoiMSJ9.P2PLhYPu7OgM1kXe615j_13E_oDbE9Lu4hclIVsh8DkmIMWX2-yhMxf0e-LEicdCjc_e8VaSdFGU5LE--gLEwC2sH71I3ilJEfJpwvfAPzgIh04UBiFVW5YLSo1Yy9chFDQbvV13HT5SUyWl0hRRShtLRX1_aevA4aWrs5hyEj3jNtJ3Mc3G3UMqujfda3kl2tuo-XMZ-H0AtccGyohL5yg5Sgp7uLpaxlWpWoUwLJw.BwmGUQgnLk4bZfTX15D7Ltvw2Iz-akDh1ZogKg3HGPg&amp;dib_tag=se&amp;keywords=Intel+core+i9+14900K&amp;qid=1741745328&amp;sr=8-6</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>2025-03-11</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>Intel Core i9-13900K Procesador de escritorio 24 (8 núcleos P + 16 núcleos E) con gráficos integrados - desbloqueado</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Página 1 de 1  </t>
+        </is>
+      </c>
+      <c r="D68" t="inlineStr">
+        <is>
+          <t>https://m.media-amazon.com/images/I/61My4F2-XUL.__AC_SX300_SY300_QL70_ML2_.jpg</t>
+        </is>
+      </c>
+      <c r="E68" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com/-/es/i9-13900K-Procesador-escritorio-gr%C3%A1ficos-integrados/dp/B0BCF54SR1/ref=sr_1_7?dib=eyJ2IjoiMSJ9.P2PLhYPu7OgM1kXe615j_13E_oDbE9Lu4hclIVsh8DkmIMWX2-yhMxf0e-LEicdCjc_e8VaSdFGU5LE--gLEwC2sH71I3ilJEfJpwvfAPzgIh04UBiFVW5YLSo1Yy9chFDQbvV13HT5SUyWl0hRRShtLRX1_aevA4aWrs5hyEj3jNtJ3Mc3G3UMqujfda3kl2tuo-XMZ-H0AtccGyohL5yg5Sgp7uLpaxlWpWoUwLJw.BwmGUQgnLk4bZfTX15D7Ltvw2Iz-akDh1ZogKg3HGPg&amp;dib_tag=se&amp;keywords=Intel+core+i9+14900K&amp;qid=1741745328&amp;sr=8-7</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>2025-03-11</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>Intel Core i9-14900KS Caja de 6.2 GHz, BX8071514900KS</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>US$813.22</t>
+        </is>
+      </c>
+      <c r="D69" t="inlineStr">
+        <is>
+          <t>https://m.media-amazon.com/images/I/51B+IODGvlL._AC_SY300_SX300_.jpg</t>
+        </is>
+      </c>
+      <c r="E69" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com/-/es/Intel-Core-i9-14900KS-Caja-BX8071514900KS/dp/B0CY3998PK/ref=sr_1_8?dib=eyJ2IjoiMSJ9.P2PLhYPu7OgM1kXe615j_13E_oDbE9Lu4hclIVsh8DkmIMWX2-yhMxf0e-LEicdCjc_e8VaSdFGU5LE--gLEwC2sH71I3ilJEfJpwvfAPzgIh04UBiFVW5YLSo1Yy9chFDQbvV13HT5SUyWl0hRRShtLRX1_aevA4aWrs5hyEj3jNtJ3Mc3G3UMqujfda3kl2tuo-XMZ-H0AtccGyohL5yg5Sgp7uLpaxlWpWoUwLJw.BwmGUQgnLk4bZfTX15D7Ltvw2Iz-akDh1ZogKg3HGPg&amp;dib_tag=se&amp;keywords=Intel+core+i9+14900K&amp;qid=1741745328&amp;sr=8-8</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>2025-03-11</t>
+        </is>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>INTEL 24 CORE I9-13900KF BX8071513900KF LGA1700 13ª generación 36 MB CACHE SRMBJ 36 TH</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>US$411.42</t>
+        </is>
+      </c>
+      <c r="D70" t="inlineStr">
+        <is>
+          <t>https://m.media-amazon.com/images/I/61-+pgXU1vL._AC_SY300_SX300_.jpg</t>
+        </is>
+      </c>
+      <c r="E70" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com/-/es/INTEL-I9-13900KF-BX8071513900KF-LGA1700-generaci%C3%B3n/dp/B0BCFM3CJ4/ref=sr_1_9?dib=eyJ2IjoiMSJ9.P2PLhYPu7OgM1kXe615j_13E_oDbE9Lu4hclIVsh8DkmIMWX2-yhMxf0e-LEicdCjc_e8VaSdFGU5LE--gLEwC2sH71I3ilJEfJpwvfAPzgIh04UBiFVW5YLSo1Yy9chFDQbvV13HT5SUyWl0hRRShtLRX1_aevA4aWrs5hyEj3jNtJ3Mc3G3UMqujfda3kl2tuo-XMZ-H0AtccGyohL5yg5Sgp7uLpaxlWpWoUwLJw.BwmGUQgnLk4bZfTX15D7Ltvw2Iz-akDh1ZogKg3HGPg&amp;dib_tag=se&amp;keywords=Intel+core+i9+14900K&amp;qid=1741745328&amp;sr=8-9</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>2025-03-11</t>
+        </is>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>Acer Nitro V Laptop para juegos | Procesador Intel Core i9-13900H | GPU NVIDIA GeForce RTX 4060 para portátil | Pantalla FHD IPS de 15.6 pulgadas de 144 Hz | DDR5 de 16 GB | SSD de 512 GB Gen 4 | WiFi</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>US$949.99</t>
+        </is>
+      </c>
+      <c r="D71" t="inlineStr">
+        <is>
+          <t>https://m.media-amazon.com/images/I/71F-Wcriq4L.__AC_SY300_SX300_QL70_ML2_.jpg</t>
+        </is>
+      </c>
+      <c r="E71" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com/-/es/Procesador-i9-13900H-port%C3%A1til-Pantalla-pulgadas/dp/B0D8JXHZTH/ref=sr_1_10?dib=eyJ2IjoiMSJ9.P2PLhYPu7OgM1kXe615j_13E_oDbE9Lu4hclIVsh8DkmIMWX2-yhMxf0e-LEicdCjc_e8VaSdFGU5LE--gLEwC2sH71I3ilJEfJpwvfAPzgIh04UBiFVW5YLSo1Yy9chFDQbvV13HT5SUyWl0hRRShtLRX1_aevA4aWrs5hyEj3jNtJ3Mc3G3UMqujfda3kl2tuo-XMZ-H0AtccGyohL5yg5Sgp7uLpaxlWpWoUwLJw.BwmGUQgnLk4bZfTX15D7Ltvw2Iz-akDh1ZogKg3HGPg&amp;dib_tag=se&amp;keywords=Intel+core+i9+14900K&amp;qid=1741745328&amp;sr=8-10</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>2025-03-11</t>
+        </is>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>GIGABYTE Z790 Aorus Elite AX (LGA 1700/ Intel Z790/ ATX/ DDR5/Quad M.2/PCIe 5.0/USB 3.2 Gen2X2 Tipo C/Intel WiFi 6E/LAN de 2.5GbE/Q-Flash Plus/PCIe EZ-Latch/placa base para juegos)</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Página 1 de 1  </t>
+        </is>
+      </c>
+      <c r="D72" t="inlineStr">
+        <is>
+          <t>https://m.media-amazon.com/images/I/81a48Z1GciL.__AC_SY300_SX300_QL70_ML2_.jpg</t>
+        </is>
+      </c>
+      <c r="E72" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com/-/es/GIGABYTE-Z790-AX-Q-Flash-EZ-Latch/dp/B0BH9DXY38/ref=sr_1_1?dib=eyJ2IjoiMSJ9.dMnmrBhbviGisPI9qa_HX5bwqzhI-_OMSKMKHMBU9GtCbmfQKD3yZolW2JufFAAwXEUPLzMoK5cs_fXGBVhW6q1neOz6us-1QdnpzDzoE4HK8t5goBzkqZRNCSaTpVd26OmBVlrlJD0KASFXkQk5qCmcCq-qLvoX4U2grCsXtHRswWO3Cysse8ErZvlpeusaP7lhf5ESeuXs6gbNueZaJOtsKEkJAKlBl4LFZ3-w78A.MblZF9pvaD5mgHLss-u1EdZeX1FYFbdPQnaPOcc7wKQ&amp;dib_tag=se&amp;keywords=z690+Gigabyte&amp;qid=1741745716&amp;sr=8-1</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>2025-03-11</t>
+        </is>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>GIGABYTE Z690 AERO G DDR4 (LGA 1700/Intel Z690/ATX/ DDR4/Quad M.2/PCIe 5.0/USB 3.2 Gen2X2 Tipo C/WiFi 6/Intel 2.5 GbE LAN/Placa base)</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>US$209.99</t>
+        </is>
+      </c>
+      <c r="D73" t="inlineStr">
+        <is>
+          <t>https://m.media-amazon.com/images/I/814fEib8qlL.__AC_SY300_SX300_QL70_ML2_.jpg</t>
+        </is>
+      </c>
+      <c r="E73" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com/-/es/GIGABYTE-Z690-Intel-Gen2X2-Placa/dp/B09L9DY4L1/ref=sr_1_2?dib=eyJ2IjoiMSJ9.dMnmrBhbviGisPI9qa_HX5bwqzhI-_OMSKMKHMBU9GtCbmfQKD3yZolW2JufFAAwXEUPLzMoK5cs_fXGBVhW6q1neOz6us-1QdnpzDzoE4HK8t5goBzkqZRNCSaTpVd26OmBVlrlJD0KASFXkQk5qCmcCq-qLvoX4U2grCsXtHRswWO3Cysse8ErZvlpeusaP7lhf5ESeuXs6gbNueZaJOtsKEkJAKlBl4LFZ3-w78A.MblZF9pvaD5mgHLss-u1EdZeX1FYFbdPQnaPOcc7wKQ&amp;dib_tag=se&amp;keywords=z690+Gigabyte&amp;qid=1741745716&amp;sr=8-2</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>2025-03-11</t>
+        </is>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>GIGABYTE Z690 Aorus Ultra (LGA 1700/Intel Z690/ATX/DDR5/Quad M.2/PCIe 5.0/USB 3.2 Gen2X2 Tipo C/WiFi 6/2.5GbE LAN/placa base para juegos)</t>
+        </is>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>US$393.90</t>
+        </is>
+      </c>
+      <c r="D74" t="inlineStr">
+        <is>
+          <t>https://m.media-amazon.com/images/I/814wvqQu+RL._AC_SX300_SY300_.jpg</t>
+        </is>
+      </c>
+      <c r="E74" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com/-/es/GIGABYTE-Z690-Gen2X2-2-5GbE-juegos/dp/B09JZFT4SN/ref=sr_1_3?dib=eyJ2IjoiMSJ9.dMnmrBhbviGisPI9qa_HX5bwqzhI-_OMSKMKHMBU9GtCbmfQKD3yZolW2JufFAAwXEUPLzMoK5cs_fXGBVhW6q1neOz6us-1QdnpzDzoE4HK8t5goBzkqZRNCSaTpVd26OmBVlrlJD0KASFXkQk5qCmcCq-qLvoX4U2grCsXtHRswWO3Cysse8ErZvlpeusaP7lhf5ESeuXs6gbNueZaJOtsKEkJAKlBl4LFZ3-w78A.MblZF9pvaD5mgHLss-u1EdZeX1FYFbdPQnaPOcc7wKQ&amp;dib_tag=se&amp;keywords=z690+Gigabyte&amp;qid=1741745716&amp;sr=8-3</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>2025-03-11</t>
+        </is>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>GIGABYTE Z690 AERO G (LGA 1700/Intel Z690/ATX/DDR5/Quad M.2/PCIe 5.0/USB 3.2 Gen2X2 Tipo C/WiFi 6/Intel 2.5 GbE LAN/Placa base)</t>
+        </is>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>US$338.00</t>
+        </is>
+      </c>
+      <c r="D75" t="inlineStr">
+        <is>
+          <t>https://m.media-amazon.com/images/I/716X5Zww1eL.__AC_SY300_SX300_QL70_ML2_.jpg</t>
+        </is>
+      </c>
+      <c r="E75" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com/-/es/GIGABYTE-Z690-Intel-Gen2X2-Placa/dp/B083NN4MLZ/ref=sr_1_4?dib=eyJ2IjoiMSJ9.dMnmrBhbviGisPI9qa_HX5bwqzhI-_OMSKMKHMBU9GtCbmfQKD3yZolW2JufFAAwXEUPLzMoK5cs_fXGBVhW6q1neOz6us-1QdnpzDzoE4HK8t5goBzkqZRNCSaTpVd26OmBVlrlJD0KASFXkQk5qCmcCq-qLvoX4U2grCsXtHRswWO3Cysse8ErZvlpeusaP7lhf5ESeuXs6gbNueZaJOtsKEkJAKlBl4LFZ3-w78A.MblZF9pvaD5mgHLss-u1EdZeX1FYFbdPQnaPOcc7wKQ&amp;dib_tag=se&amp;keywords=z690+Gigabyte&amp;qid=1741745716&amp;sr=8-4</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>2025-03-11</t>
+        </is>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>GIGABYTE Z790 GAMING PLUS AX LGA 1700 Intel Z790 ATX placa base con DDR5, Triple M.2, PCIe 4.0, USB 3.2 Gen2 Type-C, Realtek Wi-Fi 6, Realtek LAN, Q-Flash Plus, EZ-Latch</t>
+        </is>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>US$169.99</t>
+        </is>
+      </c>
+      <c r="D76" t="inlineStr">
+        <is>
+          <t>https://m.media-amazon.com/images/I/81Ip3DnEazL.__AC_SX300_SY300_QL70_ML2_.jpg</t>
+        </is>
+      </c>
+      <c r="E76" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com/-/es/GIGABYTE-Z790-AX-Realtek-EZ-Latch/dp/B0D8WH39QJ/ref=sr_1_5?dib=eyJ2IjoiMSJ9.dMnmrBhbviGisPI9qa_HX5bwqzhI-_OMSKMKHMBU9GtCbmfQKD3yZolW2JufFAAwXEUPLzMoK5cs_fXGBVhW6q1neOz6us-1QdnpzDzoE4HK8t5goBzkqZRNCSaTpVd26OmBVlrlJD0KASFXkQk5qCmcCq-qLvoX4U2grCsXtHRswWO3Cysse8ErZvlpeusaP7lhf5ESeuXs6gbNueZaJOtsKEkJAKlBl4LFZ3-w78A.MblZF9pvaD5mgHLss-u1EdZeX1FYFbdPQnaPOcc7wKQ&amp;dib_tag=se&amp;keywords=z690+Gigabyte&amp;qid=1741745716&amp;sr=8-5</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>2025-03-11</t>
+        </is>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>GIGABYTE Z790 Gaming X AX (LGA 1700/Intel/Z790/ATX/DDR5/M.2/PCIe 5.0/USB 3.2 Gen2X2 Tipo C/Intel Wi-Fi 6E/2.5GbE LAN/Q-Flash Plus/EZ-Latch Plus/Placa base para juegos)</t>
+        </is>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>US$219.99</t>
+        </is>
+      </c>
+      <c r="D77" t="inlineStr">
+        <is>
+          <t>https://m.media-amazon.com/images/I/81B9SuZS68L.__AC_SY300_SX300_QL70_ML2_.jpg</t>
+        </is>
+      </c>
+      <c r="E77" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com/-/es/GIGABYTE-Z790-AX-Q-Flash-EZ-Latch/dp/B0BSVYXM5C/ref=sr_1_6?dib=eyJ2IjoiMSJ9.dMnmrBhbviGisPI9qa_HX5bwqzhI-_OMSKMKHMBU9GtCbmfQKD3yZolW2JufFAAwXEUPLzMoK5cs_fXGBVhW6q1neOz6us-1QdnpzDzoE4HK8t5goBzkqZRNCSaTpVd26OmBVlrlJD0KASFXkQk5qCmcCq-qLvoX4U2grCsXtHRswWO3Cysse8ErZvlpeusaP7lhf5ESeuXs6gbNueZaJOtsKEkJAKlBl4LFZ3-w78A.MblZF9pvaD5mgHLss-u1EdZeX1FYFbdPQnaPOcc7wKQ&amp;dib_tag=se&amp;keywords=z690+Gigabyte&amp;qid=1741745716&amp;sr=8-6</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>2025-03-11</t>
+        </is>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>GIGABYTE Z790 UD AC (LGA 1700/Intel/Z790/ATX/DDR5/ Triple M.2/PCIe 5.0/USB 3.2 Gen2X2 Tipo C/Intel Wi-Fi/2.5GbE LAN/PCIe EZ-Latch/Multi-Key/placa base)</t>
+        </is>
+      </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Página 1 de 1  </t>
+        </is>
+      </c>
+      <c r="D78" t="inlineStr">
+        <is>
+          <t>https://m.media-amazon.com/images/I/81VisyZMvVL.__AC_SY300_SX300_QL70_ML2_.jpg</t>
+        </is>
+      </c>
+      <c r="E78" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com/-/es/GIGABYTE-Z790-Triple-EZ-Latch-Multi-Key/dp/B0BHTMXMRQ/ref=sr_1_7?dib=eyJ2IjoiMSJ9.dMnmrBhbviGisPI9qa_HX5bwqzhI-_OMSKMKHMBU9GtCbmfQKD3yZolW2JufFAAwXEUPLzMoK5cs_fXGBVhW6q1neOz6us-1QdnpzDzoE4HK8t5goBzkqZRNCSaTpVd26OmBVlrlJD0KASFXkQk5qCmcCq-qLvoX4U2grCsXtHRswWO3Cysse8ErZvlpeusaP7lhf5ESeuXs6gbNueZaJOtsKEkJAKlBl4LFZ3-w78A.MblZF9pvaD5mgHLss-u1EdZeX1FYFbdPQnaPOcc7wKQ&amp;dib_tag=se&amp;keywords=z690+Gigabyte&amp;qid=1741745716&amp;sr=8-7</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>2025-03-11</t>
+        </is>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>MSI PRO Z690-A WiFi DDR4 ProSeries - Placa base para juegos de computadora (ATX, Intel Core de 12ª generación, zócalo LGA 1700, DDR4, PCIe 4, CFX, ranuras M.2, Wi-Fi 6E), placas base Intel para PC</t>
+        </is>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>US$98.44</t>
+        </is>
+      </c>
+      <c r="D79" t="inlineStr">
+        <is>
+          <t>https://m.media-amazon.com/images/I/71xcIxpGPEL.__AC_SX300_SY300_QL70_ML2_.jpg</t>
+        </is>
+      </c>
+      <c r="E79" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com/-/es/PRO-Z690-WiFi-DDR4-ProSeries/dp/B09V6W8T36/ref=sr_1_8?dib=eyJ2IjoiMSJ9.dMnmrBhbviGisPI9qa_HX5bwqzhI-_OMSKMKHMBU9GtCbmfQKD3yZolW2JufFAAwXEUPLzMoK5cs_fXGBVhW6q1neOz6us-1QdnpzDzoE4HK8t5goBzkqZRNCSaTpVd26OmBVlrlJD0KASFXkQk5qCmcCq-qLvoX4U2grCsXtHRswWO3Cysse8ErZvlpeusaP7lhf5ESeuXs6gbNueZaJOtsKEkJAKlBl4LFZ3-w78A.MblZF9pvaD5mgHLss-u1EdZeX1FYFbdPQnaPOcc7wKQ&amp;dib_tag=se&amp;keywords=z690+Gigabyte&amp;qid=1741745716&amp;sr=8-8</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>2025-03-11</t>
+        </is>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>MSI PRO Z690-A DDR4 ProSeries - Placa base para juegos de computadora (ATX, Intel Core de 12ª generación, zócalo LGA 1700, DDR4, PCIe 4, CFX, M.2 Shield Frozr, HDMI, DisplayPort) placas base Intel</t>
+        </is>
+      </c>
+      <c r="C80" t="inlineStr">
+        <is>
+          <t>US$89.88</t>
+        </is>
+      </c>
+      <c r="D80" t="inlineStr">
+        <is>
+          <t>https://m.media-amazon.com/images/I/71NnFXzPIAL.__AC_SX300_SY300_QL70_ML2_.jpg</t>
+        </is>
+      </c>
+      <c r="E80" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com/-/es/MSI-PRO-Z690-DDR4-ProSeries/dp/B09SJXFDP8/ref=sr_1_9?dib=eyJ2IjoiMSJ9.dMnmrBhbviGisPI9qa_HX5bwqzhI-_OMSKMKHMBU9GtCbmfQKD3yZolW2JufFAAwXEUPLzMoK5cs_fXGBVhW6q1neOz6us-1QdnpzDzoE4HK8t5goBzkqZRNCSaTpVd26OmBVlrlJD0KASFXkQk5qCmcCq-qLvoX4U2grCsXtHRswWO3Cysse8ErZvlpeusaP7lhf5ESeuXs6gbNueZaJOtsKEkJAKlBl4LFZ3-w78A.MblZF9pvaD5mgHLss-u1EdZeX1FYFbdPQnaPOcc7wKQ&amp;dib_tag=se&amp;keywords=z690+Gigabyte&amp;qid=1741745716&amp;sr=8-9</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>2025-03-11</t>
+        </is>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>GIGABYTE Z790 AORUS PRO X (LGA 1700/ Intel/ Z790 X/ATX/ DDR5/ 5* M.2/PCIe 5.0/USB 3.2 Tipo-C/Wi-Fi 7/LAN de 5GbE/Q-Flash Plus/EZ-Latch Plus/Placa base)</t>
+        </is>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>US$329.99</t>
+        </is>
+      </c>
+      <c r="D81" t="inlineStr">
+        <is>
+          <t>https://m.media-amazon.com/images/I/71lzIrBDJtL.__AC_SY300_SX300_QL70_ML2_.jpg</t>
+        </is>
+      </c>
+      <c r="E81" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com/-/es/GIGABYTE-Z790-AORUS-PRO-EZ-Latch/dp/B083RW9TJF/ref=sr_1_10?dib=eyJ2IjoiMSJ9.dMnmrBhbviGisPI9qa_HX5bwqzhI-_OMSKMKHMBU9GtCbmfQKD3yZolW2JufFAAwXEUPLzMoK5cs_fXGBVhW6q1neOz6us-1QdnpzDzoE4HK8t5goBzkqZRNCSaTpVd26OmBVlrlJD0KASFXkQk5qCmcCq-qLvoX4U2grCsXtHRswWO3Cysse8ErZvlpeusaP7lhf5ESeuXs6gbNueZaJOtsKEkJAKlBl4LFZ3-w78A.MblZF9pvaD5mgHLss-u1EdZeX1FYFbdPQnaPOcc7wKQ&amp;dib_tag=se&amp;keywords=z690+Gigabyte&amp;qid=1741745716&amp;sr=8-10</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>2025-03-11</t>
+        </is>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>MSI Placa base para juegos MPG Z790 Edge WiFi (compatible con procesadores Intel de 12ª/13ª/14ª generación, LGA 1700, DDR5, PCIe 5.0, M.2, LAN de 2.5Gbps, USB 3.2 Gen2, Wi-Fi 6E, Bluetooth 5.3, ATX)</t>
+        </is>
+      </c>
+      <c r="C82" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Página 1 de 1  </t>
+        </is>
+      </c>
+      <c r="D82" t="inlineStr">
+        <is>
+          <t>https://m.media-amazon.com/images/I/81g473bLYvL.__AC_SY300_SX300_QL70_ML2_.jpg</t>
+        </is>
+      </c>
+      <c r="E82" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com/-/es/MPG-Z790-Edge-compatible-procesadores/dp/B0BL92SPJQ/ref=sr_1_1?dib=eyJ2IjoiMSJ9.hNqxVKFK6JEu3kQlOrpmtdDH1gjDQpvYgHwmmKnqcWz7al_YvSrt7viYGdR6OrVTwj--3sfh6C64i85_LKuQJt7zsVAUzTapaqhlHOXLzru3VUqw8dNfjAH0Q04rXywQ0A9-B9pYxzi7-OqWNqgP08EIBoNXqUCDEbsuW_pXGdJ_dfSkh0tuUtr21DCRbxqFmD3AwsbnerByCjwHz6BUp_F6sUMXtwqmtk87XGesRt8.hglbwXNZyDeusv4QCVGAnoIzwDaibLFls4QePmVWjmc&amp;dib_tag=se&amp;keywords=Z790+MSI&amp;qid=1741747225&amp;sr=8-1</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>2025-03-11</t>
+        </is>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>MSI PRO Z790-P WiFi ProSeries Placa base (compatible con procesadores Intel de 12ª/13ª/14ª generación, LGA 1700, DDR5, PCIe 5.0, M.2, LAN de 2.5Gbps, USB 3.2 Gen2, HDMI/DP, Wi-Fi 6E, Bluetooth 5.3,</t>
+        </is>
+      </c>
+      <c r="C83" t="inlineStr">
+        <is>
+          <t>US$169.00</t>
+        </is>
+      </c>
+      <c r="D83" t="inlineStr">
+        <is>
+          <t>https://m.media-amazon.com/images/I/81qbq1OEb7L.__AC_SY300_SX300_QL70_ML2_.jpg</t>
+        </is>
+      </c>
+      <c r="E83" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com/-/es/Z790-P-ProSeries-compatible-procesadores-generaci%C3%B3n/dp/B0BHBP8CS2/ref=sr_1_2?dib=eyJ2IjoiMSJ9.hNqxVKFK6JEu3kQlOrpmtdDH1gjDQpvYgHwmmKnqcWz7al_YvSrt7viYGdR6OrVTwj--3sfh6C64i85_LKuQJt7zsVAUzTapaqhlHOXLzru3VUqw8dNfjAH0Q04rXywQ0A9-B9pYxzi7-OqWNqgP08EIBoNXqUCDEbsuW_pXGdJ_dfSkh0tuUtr21DCRbxqFmD3AwsbnerByCjwHz6BUp_F6sUMXtwqmtk87XGesRt8.hglbwXNZyDeusv4QCVGAnoIzwDaibLFls4QePmVWjmc&amp;dib_tag=se&amp;keywords=Z790+MSI&amp;qid=1741747225&amp;sr=8-2</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>2025-03-11</t>
+        </is>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>MSI Placa base para juegos MPG Z790 Carbon WiFi II (compatible con procesadores Intel de 12ª/13ª/14ª generación, LGA 1700, DDR5, PCIe 5.0, M.2, LAN de 2.5Gbps, USB 3.2 Gen2, Wi-Fi 7, Bluetooth 5.4,</t>
+        </is>
+      </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Página 1 de 1  </t>
+        </is>
+      </c>
+      <c r="D84" t="inlineStr">
+        <is>
+          <t>https://m.media-amazon.com/images/I/91g-akagILL.__AC_SY300_SX300_QL70_ML2_.jpg</t>
+        </is>
+      </c>
+      <c r="E84" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com/-/es/Z790-II-compatible-procesadores-generaci%C3%B3n/dp/B0CTKSFD2X/ref=sr_1_3?dib=eyJ2IjoiMSJ9.hNqxVKFK6JEu3kQlOrpmtdDH1gjDQpvYgHwmmKnqcWz7al_YvSrt7viYGdR6OrVTwj--3sfh6C64i85_LKuQJt7zsVAUzTapaqhlHOXLzru3VUqw8dNfjAH0Q04rXywQ0A9-B9pYxzi7-OqWNqgP08EIBoNXqUCDEbsuW_pXGdJ_dfSkh0tuUtr21DCRbxqFmD3AwsbnerByCjwHz6BUp_F6sUMXtwqmtk87XGesRt8.hglbwXNZyDeusv4QCVGAnoIzwDaibLFls4QePmVWjmc&amp;dib_tag=se&amp;keywords=Z790+MSI&amp;qid=1741747225&amp;sr=8-3</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>2025-03-11</t>
+        </is>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>MSI MAG Z790 Tomahawk WiFi Gaming Placa base (compatible con procesadores Intel de 12ª/13ª/14ª generación, LGA 1700, DDR5, PCIe 5.0, M.2, LAN de 2.5Gbps, USB 3.2 Gen2, HDMI/DP, Wi-Fi 6E, Bluetooth</t>
+        </is>
+      </c>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Página 1 de 1  </t>
+        </is>
+      </c>
+      <c r="D85" t="inlineStr">
+        <is>
+          <t>https://m.media-amazon.com/images/I/81aRnPKw8TL.__AC_SY300_SX300_QL70_ML2_.jpg</t>
+        </is>
+      </c>
+      <c r="E85" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com/-/es/MAG-Z790-compatible-procesadores-generaci%C3%B3n/dp/B0BL8K1YH1/ref=sr_1_4?dib=eyJ2IjoiMSJ9.hNqxVKFK6JEu3kQlOrpmtdDH1gjDQpvYgHwmmKnqcWz7al_YvSrt7viYGdR6OrVTwj--3sfh6C64i85_LKuQJt7zsVAUzTapaqhlHOXLzru3VUqw8dNfjAH0Q04rXywQ0A9-B9pYxzi7-OqWNqgP08EIBoNXqUCDEbsuW_pXGdJ_dfSkh0tuUtr21DCRbxqFmD3AwsbnerByCjwHz6BUp_F6sUMXtwqmtk87XGesRt8.hglbwXNZyDeusv4QCVGAnoIzwDaibLFls4QePmVWjmc&amp;dib_tag=se&amp;keywords=Z790+MSI&amp;qid=1741747225&amp;sr=8-4</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>2025-03-11</t>
+        </is>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>MSI PRO Z790-P WiFi ProSeries Placa base (compatible con procesadores Intel de 12ª/13ª/14ª generación, LGA 1700, DDR5, PCIe 5.0, M.2, LAN de 2.5Gbps, USB 3.2 Gen2, HDMI/DP, Wi-Fi 6E, Bluetooth 5.3,</t>
+        </is>
+      </c>
+      <c r="C86" t="inlineStr">
+        <is>
+          <t>US$134.00</t>
+        </is>
+      </c>
+      <c r="D86" t="inlineStr">
+        <is>
+          <t>https://m.media-amazon.com/images/I/61+u8uf+bNL._AC_SY300_SX300_.jpg</t>
+        </is>
+      </c>
+      <c r="E86" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com/-/es/PRO-Z790-P-WiFi-ProSeries-procesadores/dp/B0DF5WNFJ2/ref=sr_1_5?dib=eyJ2IjoiMSJ9.hNqxVKFK6JEu3kQlOrpmtdDH1gjDQpvYgHwmmKnqcWz7al_YvSrt7viYGdR6OrVTwj--3sfh6C64i85_LKuQJt7zsVAUzTapaqhlHOXLzru3VUqw8dNfjAH0Q04rXywQ0A9-B9pYxzi7-OqWNqgP08EIBoNXqUCDEbsuW_pXGdJ_dfSkh0tuUtr21DCRbxqFmD3AwsbnerByCjwHz6BUp_F6sUMXtwqmtk87XGesRt8.hglbwXNZyDeusv4QCVGAnoIzwDaibLFls4QePmVWjmc&amp;dib_tag=se&amp;keywords=Z790+MSI&amp;qid=1741747225&amp;sr=8-5</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>2025-03-11</t>
+        </is>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>MSI MEG Z790 GODLIKE - Placa base para juegos (compatible con procesadores Intel de 12ª/13ª/14ª generación, LGA 1700, DDR5, PCIe 5.0, M.2, LAN de 10 Gbps, USB 3.2 Gen2, Wi-Fi 6E, Bluetooth 5.3,</t>
+        </is>
+      </c>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t>US$559.99</t>
+        </is>
+      </c>
+      <c r="D87" t="inlineStr">
+        <is>
+          <t>https://m.media-amazon.com/images/I/81R1rbU0BNL.__AC_SY300_SX300_QL70_ML2_.jpg</t>
+        </is>
+      </c>
+      <c r="E87" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com/-/es/MSI-MEG-Z790-GODLIKE-procesadores/dp/B0BL9TSHBJ/ref=sr_1_6?dib=eyJ2IjoiMSJ9.hNqxVKFK6JEu3kQlOrpmtdDH1gjDQpvYgHwmmKnqcWz7al_YvSrt7viYGdR6OrVTwj--3sfh6C64i85_LKuQJt7zsVAUzTapaqhlHOXLzru3VUqw8dNfjAH0Q04rXywQ0A9-B9pYxzi7-OqWNqgP08EIBoNXqUCDEbsuW_pXGdJ_dfSkh0tuUtr21DCRbxqFmD3AwsbnerByCjwHz6BUp_F6sUMXtwqmtk87XGesRt8.hglbwXNZyDeusv4QCVGAnoIzwDaibLFls4QePmVWjmc&amp;dib_tag=se&amp;keywords=Z790+MSI&amp;qid=1741747225&amp;sr=8-6</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>2025-03-11</t>
+        </is>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>MSI PRO Z790-P WiFi DDR4 ProSeries Placa base (compatible con procesadores Intel de 12ª/13ª/14ª generación, LGA 1700, DDR4, PCIe 5.0, M.2, LAN de 2.5Gbps, USB 3.2 Gen2, HDMI/DP, Wi-Fi 6E, Bluetooth</t>
+        </is>
+      </c>
+      <c r="C88" t="inlineStr">
+        <is>
+          <t>US$178.00</t>
+        </is>
+      </c>
+      <c r="D88" t="inlineStr">
+        <is>
+          <t>https://m.media-amazon.com/images/I/91hDAaIPbSL.__AC_SY300_SX300_QL70_ML2_.jpg</t>
+        </is>
+      </c>
+      <c r="E88" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com/-/es/Z790-P-DDR4-compatible-procesadores-generaci%C3%B3n/dp/B0BHC2LNBF/ref=sr_1_7?dib=eyJ2IjoiMSJ9.hNqxVKFK6JEu3kQlOrpmtdDH1gjDQpvYgHwmmKnqcWz7al_YvSrt7viYGdR6OrVTwj--3sfh6C64i85_LKuQJt7zsVAUzTapaqhlHOXLzru3VUqw8dNfjAH0Q04rXywQ0A9-B9pYxzi7-OqWNqgP08EIBoNXqUCDEbsuW_pXGdJ_dfSkh0tuUtr21DCRbxqFmD3AwsbnerByCjwHz6BUp_F6sUMXtwqmtk87XGesRt8.hglbwXNZyDeusv4QCVGAnoIzwDaibLFls4QePmVWjmc&amp;dib_tag=se&amp;keywords=Z790+MSI&amp;qid=1741747225&amp;sr=8-7</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>2025-03-11</t>
+        </is>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>MSI PRO Z790-A WiFi ProSeries Placa base (compatible con procesadores Intel de 12ª/13ª generación, LGA 1700, DDR5, PCIe 5.0, M.2, LAN de 2.5Gbps, USB 3.2 Gen2, Wi-Fi 6E, ATX) (renovada)</t>
+        </is>
+      </c>
+      <c r="C89" t="inlineStr">
+        <is>
+          <t>US$149.88</t>
+        </is>
+      </c>
+      <c r="D89" t="inlineStr">
+        <is>
+          <t>https://m.media-amazon.com/images/I/91z3fqxkfvL.__AC_SY300_SX300_QL70_ML2_.jpg</t>
+        </is>
+      </c>
+      <c r="E89" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com/-/es/ProSeries-compatible-procesadores-generaci%C3%B3n-renovada/dp/B0CPMFG4DS/ref=sr_1_8?dib=eyJ2IjoiMSJ9.hNqxVKFK6JEu3kQlOrpmtdDH1gjDQpvYgHwmmKnqcWz7al_YvSrt7viYGdR6OrVTwj--3sfh6C64i85_LKuQJt7zsVAUzTapaqhlHOXLzru3VUqw8dNfjAH0Q04rXywQ0A9-B9pYxzi7-OqWNqgP08EIBoNXqUCDEbsuW_pXGdJ_dfSkh0tuUtr21DCRbxqFmD3AwsbnerByCjwHz6BUp_F6sUMXtwqmtk87XGesRt8.hglbwXNZyDeusv4QCVGAnoIzwDaibLFls4QePmVWjmc&amp;dib_tag=se&amp;keywords=Z790+MSI&amp;qid=1741747225&amp;sr=8-8</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>2025-03-11</t>
+        </is>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>ASUS TUF Gaming Z790-Plus WiFi LGA 1700 (Intel 14ª, 12ª y 13ª generación) ATX placa base para juegos (PCIe 5.0, DDR5, 4xM.2 ranuras, 16+1 DrMOS, WiFi 6, LAN de 2.5 Gb, USB frontal 3.2 Gen 2 tipo C,</t>
+        </is>
+      </c>
+      <c r="C90" t="inlineStr">
+        <is>
+          <t>US$199.00</t>
+        </is>
+      </c>
+      <c r="D90" t="inlineStr">
+        <is>
+          <t>https://m.media-amazon.com/images/I/81rX0VhoStL.__AC_SX300_SY300_QL70_ML2_.jpg</t>
+        </is>
+      </c>
+      <c r="E90" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com/-/es/TUF-Z790-Plus-generaci%C3%B3n-ranuras-frontal/dp/B0BQD58D96/ref=sr_1_9?dib=eyJ2IjoiMSJ9.hNqxVKFK6JEu3kQlOrpmtdDH1gjDQpvYgHwmmKnqcWz7al_YvSrt7viYGdR6OrVTwj--3sfh6C64i85_LKuQJt7zsVAUzTapaqhlHOXLzru3VUqw8dNfjAH0Q04rXywQ0A9-B9pYxzi7-OqWNqgP08EIBoNXqUCDEbsuW_pXGdJ_dfSkh0tuUtr21DCRbxqFmD3AwsbnerByCjwHz6BUp_F6sUMXtwqmtk87XGesRt8.hglbwXNZyDeusv4QCVGAnoIzwDaibLFls4QePmVWjmc&amp;dib_tag=se&amp;keywords=Z790+MSI&amp;qid=1741747225&amp;sr=8-9</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>2025-03-11</t>
+        </is>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>GIGABYTE Z790 Aorus Elite AX (LGA 1700/ Intel Z790/ ATX/ DDR5/Quad M.2/PCIe 5.0/USB 3.2 Gen2X2 Tipo C/Intel WiFi 6E/LAN de 2.5GbE/Q-Flash Plus/PCIe EZ-Latch/placa base para juegos)</t>
+        </is>
+      </c>
+      <c r="C91" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Página 1 de 1  </t>
+        </is>
+      </c>
+      <c r="D91" t="inlineStr">
+        <is>
+          <t>https://m.media-amazon.com/images/I/81a48Z1GciL.__AC_SY300_SX300_QL70_ML2_.jpg</t>
+        </is>
+      </c>
+      <c r="E91" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com/-/es/GIGABYTE-Z790-AX-Q-Flash-EZ-Latch/dp/B0BH9DXY38/ref=sr_1_10?dib=eyJ2IjoiMSJ9.hNqxVKFK6JEu3kQlOrpmtdDH1gjDQpvYgHwmmKnqcWz7al_YvSrt7viYGdR6OrVTwj--3sfh6C64i85_LKuQJt7zsVAUzTapaqhlHOXLzru3VUqw8dNfjAH0Q04rXywQ0A9-B9pYxzi7-OqWNqgP08EIBoNXqUCDEbsuW_pXGdJ_dfSkh0tuUtr21DCRbxqFmD3AwsbnerByCjwHz6BUp_F6sUMXtwqmtk87XGesRt8.hglbwXNZyDeusv4QCVGAnoIzwDaibLFls4QePmVWjmc&amp;dib_tag=se&amp;keywords=Z790+MSI&amp;qid=1741747225&amp;sr=8-10</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>